<commit_message>
Added ELO Delta causal effect to score
</commit_message>
<xml_diff>
--- a/output/Bracket1.xlsx
+++ b/output/Bracket1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-23148" yWindow="2400" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12120" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team_Links" sheetId="1" state="visible" r:id="rId1"/>
@@ -2207,161 +2207,161 @@
     <xf numFmtId="0" fontId="46" fillId="7" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="6" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="6" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="65" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="46" fillId="7" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -2403,6 +2403,9 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom"/>
@@ -2431,9 +2434,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2575,7 +2575,7 @@
     <tableColumn id="2" uniqueName="2" name="School" queryTableFieldId="2" dataDxfId="9"/>
     <tableColumn id="3" uniqueName="3" name="Link" queryTableFieldId="3" dataDxfId="8"/>
     <tableColumn id="4" uniqueName="4" name="GameLogs" queryTableFieldId="4" dataDxfId="7"/>
-    <tableColumn id="6" uniqueName="6" name="PartialLink" queryTableFieldId="6" dataDxfId="6">
+    <tableColumn id="6" uniqueName="6" name="PartialLink" queryTableFieldId="6" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.TEXTSPLIT(
 _xlfn.TEXTSPLIT(Team_Links[[#This Row],[GameLogs]],"https://www.sports-reference.com/cbb/schools/",,TRUE,0,), "/",,TRUE,0)</calculatedColumnFormula>
     </tableColumn>
@@ -2585,7 +2585,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Teams" displayName="Teams" ref="A1:E65" headerRowCount="1" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Teams" displayName="Teams" ref="A1:E65" headerRowCount="1" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5" dataCellStyle="Normal">
   <autoFilter ref="A1:E65">
     <filterColumn colId="0" hiddenButton="1" showButton="1"/>
     <filterColumn colId="1" hiddenButton="1" showButton="1"/>
@@ -2594,13 +2594,13 @@
     <filterColumn colId="4" hiddenButton="1" showButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Seed" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Region" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Seed" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Region" dataDxfId="3" dataCellStyle="Normal"/>
     <tableColumn id="2" name="Team" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="Hyperlink Name" dataDxfId="1">
+    <tableColumn id="5" name="Hyperlink Name" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Teams[[#This Row],[Team]],Team_Links[School],Team_Links[PartialLink],,0,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Logo" dataDxfId="0" dataCellStyle="Normal">
+    <tableColumn id="4" name="Logo" dataDxfId="1" dataCellStyle="Normal">
       <calculatedColumnFormula>_xlfn.IMAGE(_xlfn.CONCAT("https://cdn.ssref.net/req/202510241/tlogo/ncaa/",TEXT(Teams[[#This Row],[Hyperlink Name]],),"-2025.png"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2902,8 +2902,8 @@
   </sheetPr>
   <dimension ref="A1:E366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>
@@ -12088,8 +12088,8 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.8" customHeight="1"/>
@@ -13618,10 +13618,10 @@
   </sheetPr>
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1"/>
@@ -13645,7 +13645,7 @@
     <col width="3.5546875" customWidth="1" style="6" min="19" max="19"/>
     <col width="9.109375" customWidth="1" style="6" min="20" max="20"/>
     <col hidden="1" width="3.5546875" customWidth="1" style="6" min="21" max="22"/>
-    <col hidden="1" width="13" customWidth="1" style="6" min="23" max="23"/>
+    <col hidden="1" style="6" min="23" max="23"/>
     <col hidden="1" width="9.109375" customWidth="1" style="6" min="24" max="16384"/>
   </cols>
   <sheetData>
@@ -18669,7 +18669,7 @@
   </sheetPr>
   <dimension ref="A1:AU69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
@@ -18723,53 +18723,53 @@
   <sheetData>
     <row r="1" ht="34.8" customFormat="1" customHeight="1" s="6">
       <c r="A1" s="13" t="n"/>
-      <c r="B1" s="279" t="inlineStr">
+      <c r="B1" s="281" t="inlineStr">
         <is>
           <t>2026 NCAA Basketball Tournament Bracket</t>
         </is>
       </c>
-      <c r="AO1" s="277" t="n"/>
+      <c r="AO1" s="287" t="n"/>
     </row>
     <row r="2" ht="19.2" customFormat="1" customHeight="1" s="63">
       <c r="A2" s="60" t="n"/>
-      <c r="B2" s="281" t="n"/>
-      <c r="C2" s="281" t="inlineStr">
+      <c r="B2" s="285" t="n"/>
+      <c r="C2" s="285" t="inlineStr">
         <is>
           <t>First Round</t>
         </is>
       </c>
-      <c r="D2" s="281" t="n"/>
+      <c r="D2" s="285" t="n"/>
       <c r="E2" s="62" t="n"/>
-      <c r="F2" s="281" t="inlineStr">
+      <c r="F2" s="285" t="inlineStr">
         <is>
           <t>Second Round</t>
         </is>
       </c>
-      <c r="G2" s="281" t="n"/>
+      <c r="G2" s="285" t="n"/>
       <c r="H2" s="62" t="n"/>
-      <c r="I2" s="281" t="inlineStr">
+      <c r="I2" s="285" t="inlineStr">
         <is>
           <t>Sweet 16</t>
         </is>
       </c>
-      <c r="J2" s="281" t="n"/>
+      <c r="J2" s="285" t="n"/>
       <c r="K2" s="62" t="n"/>
-      <c r="L2" s="281" t="inlineStr">
+      <c r="L2" s="285" t="inlineStr">
         <is>
           <t>Elite 8</t>
         </is>
       </c>
-      <c r="M2" s="281" t="n"/>
+      <c r="M2" s="285" t="n"/>
       <c r="N2" s="62" t="n"/>
-      <c r="O2" s="281" t="inlineStr">
+      <c r="O2" s="285" t="inlineStr">
         <is>
           <t>Final Four</t>
         </is>
       </c>
-      <c r="P2" s="281" t="n"/>
+      <c r="P2" s="285" t="n"/>
       <c r="Q2" s="62" t="n"/>
       <c r="R2" s="62" t="n"/>
-      <c r="S2" s="281" t="inlineStr">
+      <c r="S2" s="285" t="inlineStr">
         <is>
           <t>Championship</t>
         </is>
@@ -18777,38 +18777,38 @@
       <c r="X2" s="62" t="n"/>
       <c r="Y2" s="62" t="n"/>
       <c r="Z2" s="62" t="n"/>
-      <c r="AA2" s="281" t="inlineStr">
+      <c r="AA2" s="285" t="inlineStr">
         <is>
           <t>Final Four</t>
         </is>
       </c>
       <c r="AB2" s="62" t="n"/>
       <c r="AC2" s="62" t="n"/>
-      <c r="AD2" s="281" t="inlineStr">
+      <c r="AD2" s="285" t="inlineStr">
         <is>
           <t>Elite 8</t>
         </is>
       </c>
       <c r="AE2" s="62" t="n"/>
       <c r="AF2" s="62" t="n"/>
-      <c r="AG2" s="281" t="inlineStr">
+      <c r="AG2" s="285" t="inlineStr">
         <is>
           <t>Sweet 16</t>
         </is>
       </c>
       <c r="AH2" s="62" t="n"/>
       <c r="AI2" s="62" t="n"/>
-      <c r="AJ2" s="281">
+      <c r="AJ2" s="285">
         <f>F2</f>
         <v/>
       </c>
       <c r="AK2" s="62" t="n"/>
       <c r="AL2" s="62" t="n"/>
-      <c r="AM2" s="281">
+      <c r="AM2" s="285">
         <f>C2</f>
         <v/>
       </c>
-      <c r="AN2" s="281" t="n"/>
+      <c r="AN2" s="285" t="n"/>
       <c r="AO2" s="43" t="n"/>
       <c r="AQ2" s="64" t="n"/>
       <c r="AU2" s="65" t="inlineStr">
@@ -18835,13 +18835,13 @@
       <c r="O3" s="22" t="n"/>
       <c r="P3" s="22" t="n"/>
       <c r="Q3" s="44" t="n"/>
-      <c r="R3" s="292" t="n"/>
+      <c r="R3" s="261" t="n"/>
       <c r="S3" s="22" t="n"/>
       <c r="T3" s="52" t="n"/>
       <c r="U3" s="74" t="n"/>
       <c r="V3" s="52" t="n"/>
       <c r="W3" s="22" t="n"/>
-      <c r="X3" s="292" t="n"/>
+      <c r="X3" s="261" t="n"/>
       <c r="Y3" s="44" t="n"/>
       <c r="Z3" s="44" t="n"/>
       <c r="AA3" s="22" t="n"/>
@@ -18858,8 +18858,8 @@
       <c r="AL3" s="78" t="n"/>
       <c r="AM3" s="22" t="n"/>
       <c r="AN3" s="22" t="n"/>
-      <c r="AO3" s="277" t="n"/>
-      <c r="AQ3" s="275" t="n"/>
+      <c r="AO3" s="287" t="n"/>
+      <c r="AQ3" s="288" t="n"/>
       <c r="AU3" s="7" t="inlineStr">
         <is>
           <t>x</t>
@@ -18868,7 +18868,7 @@
     </row>
     <row r="4" ht="9.75" customHeight="1">
       <c r="A4" s="13" t="n"/>
-      <c r="B4" s="286" t="n"/>
+      <c r="B4" s="255" t="n"/>
       <c r="C4" s="34" t="n"/>
       <c r="D4" s="69" t="n"/>
       <c r="F4" s="25" t="n"/>
@@ -18891,11 +18891,11 @@
       <c r="AG4" s="25" t="n"/>
       <c r="AJ4" s="25" t="n"/>
       <c r="AM4" s="26" t="n"/>
-      <c r="AN4" s="286" t="n"/>
-      <c r="AO4" s="277" t="n"/>
+      <c r="AN4" s="255" t="n"/>
+      <c r="AO4" s="287" t="n"/>
     </row>
     <row r="5" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A5" s="278" t="n"/>
+      <c r="A5" s="286" t="n"/>
       <c r="B5" s="27" t="n">
         <v>1</v>
       </c>
@@ -18911,11 +18911,11 @@
         <f>Games!L5</f>
         <v/>
       </c>
-      <c r="F5" s="257">
+      <c r="F5" s="263">
         <f>Games!O5</f>
         <v/>
       </c>
-      <c r="G5" s="260">
+      <c r="G5" s="248">
         <f>_xlfn.XLOOKUP(F5,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -18943,11 +18943,11 @@
         <f>Games!L46</f>
         <v/>
       </c>
-      <c r="AI5" s="248">
+      <c r="AI5" s="298">
         <f>_xlfn.XLOOKUP(AJ5,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ5" s="257">
+      <c r="AJ5" s="263">
         <f>Games!O21</f>
         <v/>
       </c>
@@ -18966,14 +18966,14 @@
       <c r="AN5" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="AO5" s="277" t="n"/>
+      <c r="AO5" s="287" t="n"/>
       <c r="AU5" s="2">
         <f>IF(AP29="x",TRUE,FALSE)</f>
         <v/>
       </c>
     </row>
     <row r="6" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A6" s="255">
+      <c r="A6" s="283">
         <f>IF($AU$5=TRUE,1,"")</f>
         <v/>
       </c>
@@ -19006,7 +19006,7 @@
       <c r="AK6" s="55" t="n"/>
       <c r="AM6" s="39" t="n"/>
       <c r="AN6" s="28" t="n"/>
-      <c r="AO6" s="277">
+      <c r="AO6" s="287">
         <f>IF($AU$5=TRUE,A66+1,"")</f>
         <v/>
       </c>
@@ -19027,17 +19027,17 @@
         <f>Games!N5</f>
         <v/>
       </c>
-      <c r="F7" s="276">
+      <c r="F7" s="282">
         <f>IF($AU$5=TRUE,AO66+1,"")</f>
         <v/>
       </c>
-      <c r="G7" s="276" t="n"/>
+      <c r="G7" s="282" t="n"/>
       <c r="H7" s="49" t="n"/>
-      <c r="I7" s="264">
+      <c r="I7" s="280">
         <f>Games!O38</f>
         <v/>
       </c>
-      <c r="J7" s="260">
+      <c r="J7" s="248">
         <f>_xlfn.XLOOKUP(I7,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19062,17 +19062,17 @@
         <f>Games!L59</f>
         <v/>
       </c>
-      <c r="AF7" s="248">
+      <c r="AF7" s="298">
         <f>_xlfn.XLOOKUP(AG7,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG7" s="257">
+      <c r="AG7" s="263">
         <f>Games!O46</f>
         <v/>
       </c>
       <c r="AH7" s="55" t="n"/>
       <c r="AI7" s="51" t="n"/>
-      <c r="AJ7" s="276">
+      <c r="AJ7" s="282">
         <f>IF($AU$5=TRUE,F63+1,"")</f>
         <v/>
       </c>
@@ -19093,11 +19093,11 @@
       </c>
     </row>
     <row r="8" ht="10.2" customHeight="1" thickBot="1">
-      <c r="A8" s="278" t="n"/>
+      <c r="A8" s="286" t="n"/>
       <c r="B8" s="28" t="n"/>
       <c r="C8" s="38" t="n"/>
       <c r="D8" s="71" t="n"/>
-      <c r="G8" s="255" t="n"/>
+      <c r="G8" s="283" t="n"/>
       <c r="H8" s="50" t="n"/>
       <c r="I8" s="302" t="n"/>
       <c r="J8" s="307" t="n"/>
@@ -19121,10 +19121,10 @@
       <c r="AH8" s="56" t="n"/>
       <c r="AM8" s="39" t="n"/>
       <c r="AN8" s="28" t="n"/>
-      <c r="AO8" s="277" t="n"/>
+      <c r="AO8" s="287" t="n"/>
     </row>
     <row r="9" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A9" s="278" t="n"/>
+      <c r="A9" s="286" t="n"/>
       <c r="B9" s="27" t="n">
         <v>8</v>
       </c>
@@ -19140,11 +19140,11 @@
         <f>Games!L6</f>
         <v/>
       </c>
-      <c r="F9" s="257">
+      <c r="F9" s="263">
         <f>Games!O6</f>
         <v/>
       </c>
-      <c r="G9" s="260">
+      <c r="G9" s="248">
         <f>_xlfn.XLOOKUP(F9,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19152,8 +19152,8 @@
         <f>Games!N38</f>
         <v/>
       </c>
-      <c r="I9" s="286" t="n"/>
-      <c r="J9" s="286" t="n"/>
+      <c r="I9" s="255" t="n"/>
+      <c r="J9" s="255" t="n"/>
       <c r="K9" s="49" t="n"/>
       <c r="L9" s="25" t="n"/>
       <c r="M9" s="25" t="n"/>
@@ -19169,16 +19169,16 @@
       <c r="AA9" s="25" t="n"/>
       <c r="AD9" s="25" t="n"/>
       <c r="AE9" s="55" t="n"/>
-      <c r="AG9" s="286" t="n"/>
+      <c r="AG9" s="255" t="n"/>
       <c r="AH9" s="59">
         <f>Games!N46</f>
         <v/>
       </c>
-      <c r="AI9" s="248">
+      <c r="AI9" s="298">
         <f>_xlfn.XLOOKUP(AJ9,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ9" s="257">
+      <c r="AJ9" s="263">
         <f>Games!O22</f>
         <v/>
       </c>
@@ -19197,10 +19197,10 @@
       <c r="AN9" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="AO9" s="277" t="n"/>
+      <c r="AO9" s="287" t="n"/>
     </row>
     <row r="10" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A10" s="278">
+      <c r="A10" s="286">
         <f>IF($AU$5=TRUE,A6+1,"")</f>
         <v/>
       </c>
@@ -19211,8 +19211,8 @@
       <c r="F10" s="303" t="n"/>
       <c r="G10" s="307" t="n"/>
       <c r="H10" s="311" t="n"/>
-      <c r="I10" s="286" t="n"/>
-      <c r="J10" s="286" t="n"/>
+      <c r="I10" s="255" t="n"/>
+      <c r="J10" s="255" t="n"/>
       <c r="K10" s="50" t="n"/>
       <c r="L10" s="25" t="n"/>
       <c r="M10" s="25" t="n"/>
@@ -19228,14 +19228,14 @@
       <c r="AA10" s="25" t="n"/>
       <c r="AD10" s="25" t="n"/>
       <c r="AE10" s="56" t="n"/>
-      <c r="AG10" s="286" t="n"/>
+      <c r="AG10" s="255" t="n"/>
       <c r="AH10" s="312" t="n"/>
       <c r="AI10" s="309" t="n"/>
       <c r="AJ10" s="303" t="n"/>
       <c r="AK10" s="55" t="n"/>
       <c r="AM10" s="39" t="n"/>
       <c r="AN10" s="28" t="n"/>
-      <c r="AO10" s="277">
+      <c r="AO10" s="287">
         <f>IF($AU$5=TRUE,AO6+1,"")</f>
         <v/>
       </c>
@@ -19256,19 +19256,19 @@
         <f>Games!N6</f>
         <v/>
       </c>
-      <c r="F11" s="286" t="n"/>
-      <c r="G11" s="286" t="n"/>
-      <c r="I11" s="255">
+      <c r="F11" s="255" t="n"/>
+      <c r="G11" s="255" t="n"/>
+      <c r="I11" s="283">
         <f>IF($AU$5=TRUE,AJ63+1,"")</f>
         <v/>
       </c>
-      <c r="J11" s="255" t="n"/>
+      <c r="J11" s="283" t="n"/>
       <c r="K11" s="50" t="n"/>
-      <c r="L11" s="264">
+      <c r="L11" s="280">
         <f>Games!O55</f>
         <v/>
       </c>
-      <c r="M11" s="260">
+      <c r="M11" s="248">
         <f>_xlfn.XLOOKUP(L11,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19297,16 +19297,16 @@
         <f>_xlfn.XLOOKUP(AD11,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AD11" s="257">
+      <c r="AD11" s="263">
         <f>Games!O59</f>
         <v/>
       </c>
       <c r="AE11" s="56" t="n"/>
-      <c r="AG11" s="255">
+      <c r="AG11" s="283">
         <f>IF($AU$5=TRUE,I59+1,"")</f>
         <v/>
       </c>
-      <c r="AJ11" s="286" t="n"/>
+      <c r="AJ11" s="255" t="n"/>
       <c r="AK11" s="59">
         <f>Games!N22</f>
         <v/>
@@ -19324,13 +19324,13 @@
       </c>
     </row>
     <row r="12" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A12" s="278" t="n"/>
+      <c r="A12" s="286" t="n"/>
       <c r="B12" s="28" t="n"/>
       <c r="C12" s="38" t="n"/>
       <c r="D12" s="71" t="n"/>
-      <c r="F12" s="286" t="n"/>
-      <c r="G12" s="286" t="n"/>
-      <c r="J12" s="255" t="n"/>
+      <c r="F12" s="255" t="n"/>
+      <c r="G12" s="255" t="n"/>
+      <c r="J12" s="283" t="n"/>
       <c r="K12" s="50" t="n"/>
       <c r="L12" s="302" t="n"/>
       <c r="M12" s="307" t="n"/>
@@ -19348,13 +19348,13 @@
       <c r="AC12" s="303" t="n"/>
       <c r="AD12" s="303" t="n"/>
       <c r="AE12" s="56" t="n"/>
-      <c r="AJ12" s="286" t="n"/>
+      <c r="AJ12" s="255" t="n"/>
       <c r="AM12" s="39" t="n"/>
       <c r="AN12" s="28" t="n"/>
-      <c r="AO12" s="277" t="n"/>
+      <c r="AO12" s="287" t="n"/>
     </row>
     <row r="13" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A13" s="278" t="n"/>
+      <c r="A13" s="286" t="n"/>
       <c r="B13" s="27" t="n">
         <v>5</v>
       </c>
@@ -19370,11 +19370,11 @@
         <f>Games!L7</f>
         <v/>
       </c>
-      <c r="F13" s="257">
+      <c r="F13" s="263">
         <f>Games!O7</f>
         <v/>
       </c>
-      <c r="G13" s="260">
+      <c r="G13" s="248">
         <f>_xlfn.XLOOKUP(F13,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19382,8 +19382,8 @@
         <f>Games!L39</f>
         <v/>
       </c>
-      <c r="I13" s="286" t="n"/>
-      <c r="J13" s="286" t="n"/>
+      <c r="I13" s="255" t="n"/>
+      <c r="J13" s="255" t="n"/>
       <c r="K13" s="50" t="n"/>
       <c r="L13" s="25" t="n"/>
       <c r="M13" s="25" t="n"/>
@@ -19400,7 +19400,7 @@
       <c r="AB13" s="55" t="n"/>
       <c r="AD13" s="25" t="n"/>
       <c r="AE13" s="56" t="n"/>
-      <c r="AG13" s="286" t="n"/>
+      <c r="AG13" s="255" t="n"/>
       <c r="AH13" s="58">
         <f>Games!L47</f>
         <v/>
@@ -19409,7 +19409,7 @@
         <f>_xlfn.XLOOKUP(AJ13,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ13" s="257">
+      <c r="AJ13" s="263">
         <f>Games!O23</f>
         <v/>
       </c>
@@ -19428,11 +19428,11 @@
       <c r="AN13" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="AO13" s="277" t="n"/>
+      <c r="AO13" s="287" t="n"/>
       <c r="AQ13" s="9" t="n"/>
     </row>
     <row r="14" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A14" s="255">
+      <c r="A14" s="283">
         <f>IF($AU$5=TRUE,A10+1,"")</f>
         <v/>
       </c>
@@ -19443,8 +19443,8 @@
       <c r="F14" s="303" t="n"/>
       <c r="G14" s="307" t="n"/>
       <c r="H14" s="308" t="n"/>
-      <c r="I14" s="286" t="n"/>
-      <c r="J14" s="286" t="n"/>
+      <c r="I14" s="255" t="n"/>
+      <c r="J14" s="255" t="n"/>
       <c r="K14" s="50" t="n"/>
       <c r="L14" s="25" t="n"/>
       <c r="M14" s="25" t="n"/>
@@ -19461,18 +19461,18 @@
       <c r="AB14" s="56" t="n"/>
       <c r="AD14" s="25" t="n"/>
       <c r="AE14" s="56" t="n"/>
-      <c r="AG14" s="286" t="n"/>
+      <c r="AG14" s="255" t="n"/>
       <c r="AH14" s="308" t="n"/>
       <c r="AI14" s="303" t="n"/>
       <c r="AJ14" s="303" t="n"/>
       <c r="AK14" s="55" t="n"/>
       <c r="AM14" s="39" t="n"/>
       <c r="AN14" s="28" t="n"/>
-      <c r="AO14" s="277">
+      <c r="AO14" s="287">
         <f>IF($AU$5=TRUE,AO10+1,"")</f>
         <v/>
       </c>
-      <c r="AQ14" s="275" t="n"/>
+      <c r="AQ14" s="288" t="n"/>
     </row>
     <row r="15" ht="13.8" customHeight="1" thickBot="1">
       <c r="B15" s="27" t="n">
@@ -19490,17 +19490,17 @@
         <f>Games!N7</f>
         <v/>
       </c>
-      <c r="F15" s="276">
+      <c r="F15" s="282">
         <f>IF($AU$5=TRUE,F7+1,"")</f>
         <v/>
       </c>
-      <c r="G15" s="276" t="n"/>
+      <c r="G15" s="282" t="n"/>
       <c r="H15" s="49" t="n"/>
-      <c r="I15" s="264">
+      <c r="I15" s="280">
         <f>Games!O39</f>
         <v/>
       </c>
-      <c r="J15" s="260">
+      <c r="J15" s="248">
         <f>_xlfn.XLOOKUP(I15,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19530,13 +19530,13 @@
         <f>_xlfn.XLOOKUP(AG15,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG15" s="257">
+      <c r="AG15" s="263">
         <f>Games!O47</f>
         <v/>
       </c>
       <c r="AH15" s="55" t="n"/>
       <c r="AI15" s="51" t="n"/>
-      <c r="AJ15" s="276">
+      <c r="AJ15" s="282">
         <f>IF($AU$5=TRUE,AJ7+1,"")</f>
         <v/>
       </c>
@@ -19557,11 +19557,11 @@
       </c>
     </row>
     <row r="16" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A16" s="278" t="n"/>
+      <c r="A16" s="286" t="n"/>
       <c r="B16" s="28" t="n"/>
       <c r="C16" s="38" t="n"/>
       <c r="D16" s="71" t="n"/>
-      <c r="G16" s="255" t="n"/>
+      <c r="G16" s="283" t="n"/>
       <c r="H16" s="50" t="n"/>
       <c r="I16" s="302" t="n"/>
       <c r="J16" s="307" t="n"/>
@@ -19586,10 +19586,10 @@
       <c r="AH16" s="56" t="n"/>
       <c r="AM16" s="39" t="n"/>
       <c r="AN16" s="28" t="n"/>
-      <c r="AO16" s="277" t="n"/>
+      <c r="AO16" s="287" t="n"/>
     </row>
     <row r="17" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A17" s="278" t="n"/>
+      <c r="A17" s="286" t="n"/>
       <c r="B17" s="27" t="n">
         <v>4</v>
       </c>
@@ -19605,11 +19605,11 @@
         <f>Games!L8</f>
         <v/>
       </c>
-      <c r="F17" s="257">
+      <c r="F17" s="263">
         <f>Games!O8</f>
         <v/>
       </c>
-      <c r="G17" s="260">
+      <c r="G17" s="248">
         <f>_xlfn.XLOOKUP(F17,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19617,8 +19617,8 @@
         <f>Games!N39</f>
         <v/>
       </c>
-      <c r="I17" s="286" t="n"/>
-      <c r="J17" s="286" t="n"/>
+      <c r="I17" s="255" t="n"/>
+      <c r="J17" s="255" t="n"/>
       <c r="L17" s="25" t="n"/>
       <c r="M17" s="25" t="n"/>
       <c r="N17" s="50" t="n"/>
@@ -19633,7 +19633,7 @@
       <c r="AA17" s="25" t="n"/>
       <c r="AB17" s="56" t="n"/>
       <c r="AD17" s="25" t="n"/>
-      <c r="AG17" s="286" t="n"/>
+      <c r="AG17" s="255" t="n"/>
       <c r="AH17" s="59">
         <f>Games!N47</f>
         <v/>
@@ -19642,7 +19642,7 @@
         <f>_xlfn.XLOOKUP(AJ17,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ17" s="257">
+      <c r="AJ17" s="263">
         <f>Games!O24</f>
         <v/>
       </c>
@@ -19661,10 +19661,10 @@
       <c r="AN17" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="AO17" s="277" t="n"/>
+      <c r="AO17" s="287" t="n"/>
     </row>
     <row r="18" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A18" s="255">
+      <c r="A18" s="283">
         <f>IF($AU$5=TRUE,A14+1,"")</f>
         <v/>
       </c>
@@ -19675,8 +19675,8 @@
       <c r="F18" s="303" t="n"/>
       <c r="G18" s="307" t="n"/>
       <c r="H18" s="311" t="n"/>
-      <c r="I18" s="286" t="n"/>
-      <c r="J18" s="286" t="n"/>
+      <c r="I18" s="255" t="n"/>
+      <c r="J18" s="255" t="n"/>
       <c r="L18" s="25" t="n"/>
       <c r="M18" s="25" t="n"/>
       <c r="N18" s="50" t="n"/>
@@ -19691,14 +19691,14 @@
       <c r="AA18" s="25" t="n"/>
       <c r="AB18" s="56" t="n"/>
       <c r="AD18" s="25" t="n"/>
-      <c r="AG18" s="286" t="n"/>
+      <c r="AG18" s="255" t="n"/>
       <c r="AH18" s="312" t="n"/>
       <c r="AI18" s="303" t="n"/>
       <c r="AJ18" s="303" t="n"/>
       <c r="AK18" s="55" t="n"/>
       <c r="AM18" s="39" t="n"/>
       <c r="AN18" s="28" t="n"/>
-      <c r="AO18" s="277">
+      <c r="AO18" s="287">
         <f>IF($AU$5=TRUE,AO14+1,"")</f>
         <v/>
       </c>
@@ -19719,22 +19719,22 @@
         <f>Games!N8</f>
         <v/>
       </c>
-      <c r="F19" s="286" t="n"/>
-      <c r="G19" s="286" t="n"/>
-      <c r="I19" s="286" t="n"/>
-      <c r="J19" s="286" t="n"/>
-      <c r="K19" s="258" t="inlineStr">
+      <c r="F19" s="255" t="n"/>
+      <c r="G19" s="255" t="n"/>
+      <c r="I19" s="255" t="n"/>
+      <c r="J19" s="255" t="n"/>
+      <c r="K19" s="266" t="inlineStr">
         <is>
           <t>South</t>
         </is>
       </c>
-      <c r="M19" s="258" t="n"/>
+      <c r="M19" s="266" t="n"/>
       <c r="N19" s="50" t="n"/>
-      <c r="O19" s="264">
+      <c r="O19" s="280">
         <f>Games!O64</f>
         <v/>
       </c>
-      <c r="P19" s="260">
+      <c r="P19" s="248">
         <f>_xlfn.XLOOKUP(O19,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19757,19 +19757,19 @@
         <f>_xlfn.XLOOKUP(AA19,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AA19" s="257">
+      <c r="AA19" s="263">
         <f>Games!O66</f>
         <v/>
       </c>
       <c r="AB19" s="56" t="n"/>
-      <c r="AD19" s="258" t="inlineStr">
+      <c r="AD19" s="266" t="inlineStr">
         <is>
           <t>East</t>
         </is>
       </c>
-      <c r="AF19" s="258" t="n"/>
-      <c r="AG19" s="286" t="n"/>
-      <c r="AJ19" s="286" t="n"/>
+      <c r="AF19" s="266" t="n"/>
+      <c r="AG19" s="255" t="n"/>
+      <c r="AJ19" s="255" t="n"/>
       <c r="AK19" s="59">
         <f>Games!N24</f>
         <v/>
@@ -19787,15 +19787,15 @@
       </c>
     </row>
     <row r="20" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A20" s="278" t="n"/>
+      <c r="A20" s="286" t="n"/>
       <c r="B20" s="28" t="n"/>
       <c r="C20" s="38" t="n"/>
       <c r="D20" s="71" t="n"/>
-      <c r="F20" s="286" t="n"/>
-      <c r="G20" s="286" t="n"/>
-      <c r="I20" s="286" t="n"/>
-      <c r="J20" s="286" t="n"/>
-      <c r="M20" s="258" t="n"/>
+      <c r="F20" s="255" t="n"/>
+      <c r="G20" s="255" t="n"/>
+      <c r="I20" s="255" t="n"/>
+      <c r="J20" s="255" t="n"/>
+      <c r="M20" s="266" t="n"/>
       <c r="N20" s="50" t="n"/>
       <c r="O20" s="302" t="n"/>
       <c r="P20" s="307" t="n"/>
@@ -19811,16 +19811,16 @@
       <c r="Z20" s="303" t="n"/>
       <c r="AA20" s="303" t="n"/>
       <c r="AB20" s="56" t="n"/>
-      <c r="AF20" s="258" t="n"/>
-      <c r="AG20" s="286" t="n"/>
-      <c r="AJ20" s="286" t="n"/>
+      <c r="AF20" s="266" t="n"/>
+      <c r="AG20" s="255" t="n"/>
+      <c r="AJ20" s="255" t="n"/>
       <c r="AM20" s="39" t="n"/>
       <c r="AN20" s="28" t="n"/>
-      <c r="AO20" s="277" t="n"/>
+      <c r="AO20" s="287" t="n"/>
       <c r="AQ20" s="10" t="n"/>
     </row>
     <row r="21" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A21" s="255">
+      <c r="A21" s="283">
         <f>IF($AU$5=TRUE,A18+1,"")</f>
         <v/>
       </c>
@@ -19839,11 +19839,11 @@
         <f>Games!L9</f>
         <v/>
       </c>
-      <c r="F21" s="257">
+      <c r="F21" s="263">
         <f>Games!O9</f>
         <v/>
       </c>
-      <c r="G21" s="260">
+      <c r="G21" s="248">
         <f>_xlfn.XLOOKUP(F21,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -19851,8 +19851,8 @@
         <f>Games!L40</f>
         <v/>
       </c>
-      <c r="I21" s="286" t="n"/>
-      <c r="J21" s="286" t="n"/>
+      <c r="I21" s="255" t="n"/>
+      <c r="J21" s="255" t="n"/>
       <c r="L21" s="18">
         <f>IF($AU$5=TRUE,AG59+1,"")</f>
         <v/>
@@ -19872,11 +19872,11 @@
       <c r="Y21" s="55" t="n"/>
       <c r="AA21" s="25" t="n"/>
       <c r="AB21" s="56" t="n"/>
-      <c r="AD21" s="278">
+      <c r="AD21" s="286">
         <f>IF($AU$5=TRUE,L53+1,"")</f>
         <v/>
       </c>
-      <c r="AG21" s="286" t="n"/>
+      <c r="AG21" s="255" t="n"/>
       <c r="AH21" s="58">
         <f>Games!L48</f>
         <v/>
@@ -19885,7 +19885,7 @@
         <f>_xlfn.XLOOKUP(AJ21,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ21" s="257">
+      <c r="AJ21" s="263">
         <f>Games!O25</f>
         <v/>
       </c>
@@ -19904,7 +19904,7 @@
       <c r="AN21" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="AO21" s="277" t="n"/>
+      <c r="AO21" s="287" t="n"/>
       <c r="AQ21" s="9" t="n"/>
     </row>
     <row r="22" ht="10.5" customHeight="1" thickBot="1">
@@ -19915,8 +19915,8 @@
       <c r="F22" s="303" t="n"/>
       <c r="G22" s="307" t="n"/>
       <c r="H22" s="308" t="n"/>
-      <c r="I22" s="286" t="n"/>
-      <c r="J22" s="286" t="n"/>
+      <c r="I22" s="255" t="n"/>
+      <c r="J22" s="255" t="n"/>
       <c r="L22" s="25" t="n"/>
       <c r="M22" s="25" t="n"/>
       <c r="N22" s="50" t="n"/>
@@ -19934,21 +19934,21 @@
       <c r="AA22" s="25" t="n"/>
       <c r="AB22" s="56" t="n"/>
       <c r="AD22" s="29" t="n"/>
-      <c r="AG22" s="286" t="n"/>
+      <c r="AG22" s="255" t="n"/>
       <c r="AH22" s="308" t="n"/>
       <c r="AI22" s="303" t="n"/>
       <c r="AJ22" s="303" t="n"/>
       <c r="AK22" s="55" t="n"/>
       <c r="AM22" s="39" t="n"/>
       <c r="AN22" s="28" t="n"/>
-      <c r="AO22" s="277">
+      <c r="AO22" s="287">
         <f>IF($AU$5=TRUE,AO18+1,"")</f>
         <v/>
       </c>
-      <c r="AQ22" s="275" t="n"/>
+      <c r="AQ22" s="288" t="n"/>
     </row>
     <row r="23" ht="13.8" customHeight="1" thickBot="1">
-      <c r="A23" s="278" t="n"/>
+      <c r="A23" s="286" t="n"/>
       <c r="B23" s="27" t="n">
         <v>11</v>
       </c>
@@ -19964,17 +19964,17 @@
         <f>Games!N9</f>
         <v/>
       </c>
-      <c r="F23" s="276">
+      <c r="F23" s="282">
         <f>IF($AU$5=TRUE,F15+1,"")</f>
         <v/>
       </c>
-      <c r="G23" s="276" t="n"/>
+      <c r="G23" s="282" t="n"/>
       <c r="H23" s="49" t="n"/>
-      <c r="I23" s="264">
+      <c r="I23" s="280">
         <f>Games!O40</f>
         <v/>
       </c>
-      <c r="J23" s="260">
+      <c r="J23" s="248">
         <f>_xlfn.XLOOKUP(I23,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20007,13 +20007,13 @@
         <f>_xlfn.XLOOKUP(AG23,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG23" s="257">
+      <c r="AG23" s="263">
         <f>Games!O48</f>
         <v/>
       </c>
       <c r="AH23" s="55" t="n"/>
       <c r="AI23" s="51" t="n"/>
-      <c r="AJ23" s="276">
+      <c r="AJ23" s="282">
         <f>IF($AU$5=TRUE,AJ15+1,"")</f>
         <v/>
       </c>
@@ -20034,11 +20034,11 @@
       </c>
     </row>
     <row r="24" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A24" s="278" t="n"/>
+      <c r="A24" s="286" t="n"/>
       <c r="B24" s="28" t="n"/>
       <c r="C24" s="38" t="n"/>
       <c r="D24" s="71" t="n"/>
-      <c r="G24" s="255" t="n"/>
+      <c r="G24" s="283" t="n"/>
       <c r="H24" s="50" t="n"/>
       <c r="I24" s="302" t="n"/>
       <c r="J24" s="307" t="n"/>
@@ -20066,10 +20066,10 @@
       <c r="AH24" s="56" t="n"/>
       <c r="AM24" s="39" t="n"/>
       <c r="AN24" s="28" t="n"/>
-      <c r="AO24" s="277" t="n"/>
+      <c r="AO24" s="287" t="n"/>
     </row>
     <row r="25" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A25" s="278" t="n"/>
+      <c r="A25" s="286" t="n"/>
       <c r="B25" s="27" t="n">
         <v>3</v>
       </c>
@@ -20085,11 +20085,11 @@
         <f>Games!L10</f>
         <v/>
       </c>
-      <c r="F25" s="257">
+      <c r="F25" s="263">
         <f>Games!O10</f>
         <v/>
       </c>
-      <c r="G25" s="260">
+      <c r="G25" s="248">
         <f>_xlfn.XLOOKUP(F25,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20097,8 +20097,8 @@
         <f>Games!N40</f>
         <v/>
       </c>
-      <c r="I25" s="286" t="n"/>
-      <c r="J25" s="286" t="n"/>
+      <c r="I25" s="255" t="n"/>
+      <c r="J25" s="255" t="n"/>
       <c r="K25" s="49" t="n"/>
       <c r="L25" s="25" t="n"/>
       <c r="M25" s="25" t="n"/>
@@ -20118,7 +20118,7 @@
       <c r="AB25" s="56" t="n"/>
       <c r="AD25" s="25" t="n"/>
       <c r="AE25" s="55" t="n"/>
-      <c r="AG25" s="286" t="n"/>
+      <c r="AG25" s="255" t="n"/>
       <c r="AH25" s="59">
         <f>Games!N48</f>
         <v/>
@@ -20127,7 +20127,7 @@
         <f>_xlfn.XLOOKUP(AJ25,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ25" s="257">
+      <c r="AJ25" s="263">
         <f>Games!O26</f>
         <v/>
       </c>
@@ -20146,10 +20146,10 @@
       <c r="AN25" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="AO25" s="277" t="n"/>
+      <c r="AO25" s="287" t="n"/>
     </row>
     <row r="26" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A26" s="255">
+      <c r="A26" s="283">
         <f>IF($AU$5=TRUE,A21+1,"")</f>
         <v/>
       </c>
@@ -20160,8 +20160,8 @@
       <c r="F26" s="303" t="n"/>
       <c r="G26" s="307" t="n"/>
       <c r="H26" s="311" t="n"/>
-      <c r="I26" s="286" t="n"/>
-      <c r="J26" s="286" t="n"/>
+      <c r="I26" s="255" t="n"/>
+      <c r="J26" s="255" t="n"/>
       <c r="K26" s="50" t="n"/>
       <c r="L26" s="25" t="n"/>
       <c r="M26" s="25" t="n"/>
@@ -20181,14 +20181,14 @@
       <c r="AB26" s="56" t="n"/>
       <c r="AD26" s="25" t="n"/>
       <c r="AE26" s="56" t="n"/>
-      <c r="AG26" s="286" t="n"/>
+      <c r="AG26" s="255" t="n"/>
       <c r="AH26" s="312" t="n"/>
       <c r="AI26" s="303" t="n"/>
       <c r="AJ26" s="303" t="n"/>
       <c r="AK26" s="55" t="n"/>
       <c r="AM26" s="39" t="n"/>
       <c r="AN26" s="28" t="n"/>
-      <c r="AO26" s="277">
+      <c r="AO26" s="287">
         <f>IF($AU$5=TRUE,AO22+1,"")</f>
         <v/>
       </c>
@@ -20209,19 +20209,19 @@
         <f>Games!N10</f>
         <v/>
       </c>
-      <c r="F27" s="286" t="n"/>
-      <c r="G27" s="286" t="n"/>
-      <c r="I27" s="255">
+      <c r="F27" s="255" t="n"/>
+      <c r="G27" s="255" t="n"/>
+      <c r="I27" s="283">
         <f>IF($AU$5=TRUE,I11+1,"")</f>
         <v/>
       </c>
-      <c r="J27" s="255" t="n"/>
+      <c r="J27" s="283" t="n"/>
       <c r="K27" s="50" t="n"/>
-      <c r="L27" s="264">
+      <c r="L27" s="280">
         <f>Games!O56</f>
         <v/>
       </c>
-      <c r="M27" s="260">
+      <c r="M27" s="248">
         <f>_xlfn.XLOOKUP(L27,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20232,11 +20232,11 @@
       <c r="O27" s="25" t="n"/>
       <c r="P27" s="25" t="n"/>
       <c r="Q27" s="50" t="n"/>
-      <c r="R27" s="264">
+      <c r="R27" s="280">
         <f>Games!O69</f>
         <v/>
       </c>
-      <c r="U27" s="272">
+      <c r="U27" s="290">
         <f>_xlfn.XLOOKUP(R27,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20244,7 +20244,7 @@
         <f>Games!L72</f>
         <v/>
       </c>
-      <c r="W27" s="286" t="n"/>
+      <c r="W27" s="255" t="n"/>
       <c r="X27" s="25" t="n"/>
       <c r="Y27" s="56" t="n"/>
       <c r="AA27" s="25" t="n"/>
@@ -20256,16 +20256,16 @@
         <f>_xlfn.XLOOKUP(AD27,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AD27" s="257">
+      <c r="AD27" s="263">
         <f>Games!O60</f>
         <v/>
       </c>
       <c r="AE27" s="56" t="n"/>
-      <c r="AG27" s="255">
+      <c r="AG27" s="283">
         <f>IF($AU$5=TRUE,AG11+1,"")</f>
         <v/>
       </c>
-      <c r="AJ27" s="286" t="n"/>
+      <c r="AJ27" s="255" t="n"/>
       <c r="AK27" s="59">
         <f>Games!N26</f>
         <v/>
@@ -20283,13 +20283,13 @@
       </c>
     </row>
     <row r="28" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A28" s="278" t="n"/>
+      <c r="A28" s="286" t="n"/>
       <c r="B28" s="28" t="n"/>
       <c r="C28" s="38" t="n"/>
       <c r="D28" s="71" t="n"/>
-      <c r="F28" s="286" t="n"/>
-      <c r="G28" s="286" t="n"/>
-      <c r="J28" s="255" t="n"/>
+      <c r="F28" s="255" t="n"/>
+      <c r="G28" s="255" t="n"/>
+      <c r="J28" s="283" t="n"/>
       <c r="K28" s="50" t="n"/>
       <c r="L28" s="302" t="n"/>
       <c r="M28" s="307" t="n"/>
@@ -20302,7 +20302,7 @@
       <c r="T28" s="303" t="n"/>
       <c r="U28" s="307" t="n"/>
       <c r="V28" s="308" t="n"/>
-      <c r="W28" s="286" t="n"/>
+      <c r="W28" s="255" t="n"/>
       <c r="X28" s="25" t="n"/>
       <c r="Y28" s="56" t="n"/>
       <c r="AA28" s="25" t="n"/>
@@ -20310,13 +20310,13 @@
       <c r="AC28" s="303" t="n"/>
       <c r="AD28" s="303" t="n"/>
       <c r="AE28" s="56" t="n"/>
-      <c r="AJ28" s="286" t="n"/>
+      <c r="AJ28" s="255" t="n"/>
       <c r="AM28" s="39" t="n"/>
       <c r="AN28" s="28" t="n"/>
-      <c r="AO28" s="277" t="n"/>
+      <c r="AO28" s="287" t="n"/>
     </row>
     <row r="29" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A29" s="278" t="n"/>
+      <c r="A29" s="286" t="n"/>
       <c r="B29" s="27" t="n">
         <v>7</v>
       </c>
@@ -20332,11 +20332,11 @@
         <f>Games!L11</f>
         <v/>
       </c>
-      <c r="F29" s="257">
+      <c r="F29" s="263">
         <f>Games!O11</f>
         <v/>
       </c>
-      <c r="G29" s="260">
+      <c r="G29" s="248">
         <f>_xlfn.XLOOKUP(F29,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20344,8 +20344,8 @@
         <f>Games!L41</f>
         <v/>
       </c>
-      <c r="I29" s="286" t="n"/>
-      <c r="J29" s="286" t="n"/>
+      <c r="I29" s="255" t="n"/>
+      <c r="J29" s="255" t="n"/>
       <c r="K29" s="50" t="n"/>
       <c r="L29" s="25" t="n"/>
       <c r="M29" s="25" t="n"/>
@@ -20363,7 +20363,7 @@
       <c r="AA29" s="25" t="n"/>
       <c r="AD29" s="25" t="n"/>
       <c r="AE29" s="56" t="n"/>
-      <c r="AG29" s="286" t="n"/>
+      <c r="AG29" s="255" t="n"/>
       <c r="AH29" s="58">
         <f>Games!L49</f>
         <v/>
@@ -20372,7 +20372,7 @@
         <f>_xlfn.XLOOKUP(AJ29,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ29" s="257">
+      <c r="AJ29" s="263">
         <f>Games!O27</f>
         <v/>
       </c>
@@ -20391,7 +20391,7 @@
       <c r="AN29" s="27" t="n">
         <v>7</v>
       </c>
-      <c r="AO29" s="277" t="n"/>
+      <c r="AO29" s="287" t="n"/>
       <c r="AP29" s="11" t="inlineStr">
         <is>
           <t>x</t>
@@ -20404,7 +20404,7 @@
       </c>
     </row>
     <row r="30" ht="10.2" customHeight="1" thickBot="1">
-      <c r="A30" s="255">
+      <c r="A30" s="283">
         <f>IF($AU$5=TRUE,A26+1,"")</f>
         <v/>
       </c>
@@ -20415,8 +20415,8 @@
       <c r="F30" s="303" t="n"/>
       <c r="G30" s="307" t="n"/>
       <c r="H30" s="308" t="n"/>
-      <c r="I30" s="286" t="n"/>
-      <c r="J30" s="286" t="n"/>
+      <c r="I30" s="255" t="n"/>
+      <c r="J30" s="255" t="n"/>
       <c r="K30" s="50" t="n"/>
       <c r="L30" s="25" t="n"/>
       <c r="M30" s="25" t="n"/>
@@ -20434,14 +20434,14 @@
       <c r="AA30" s="25" t="n"/>
       <c r="AD30" s="25" t="n"/>
       <c r="AE30" s="56" t="n"/>
-      <c r="AG30" s="286" t="n"/>
+      <c r="AG30" s="255" t="n"/>
       <c r="AH30" s="308" t="n"/>
       <c r="AI30" s="303" t="n"/>
       <c r="AJ30" s="303" t="n"/>
       <c r="AK30" s="55" t="n"/>
       <c r="AM30" s="39" t="n"/>
       <c r="AN30" s="28" t="n"/>
-      <c r="AO30" s="277">
+      <c r="AO30" s="287">
         <f>IF($AU$5=TRUE,AO26+1,"")</f>
         <v/>
       </c>
@@ -20462,17 +20462,17 @@
         <f>Games!N11</f>
         <v/>
       </c>
-      <c r="F31" s="276">
+      <c r="F31" s="282">
         <f>IF($AU$5=TRUE,F23+1,"")</f>
         <v/>
       </c>
-      <c r="G31" s="276" t="n"/>
+      <c r="G31" s="282" t="n"/>
       <c r="H31" s="49" t="n"/>
-      <c r="I31" s="264">
+      <c r="I31" s="280">
         <f>Games!O41</f>
         <v/>
       </c>
-      <c r="J31" s="260">
+      <c r="J31" s="248">
         <f>_xlfn.XLOOKUP(I31,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20486,7 +20486,7 @@
       <c r="P31" s="25" t="n"/>
       <c r="Q31" s="50" t="n"/>
       <c r="R31" s="4" t="n"/>
-      <c r="S31" s="286" t="inlineStr">
+      <c r="S31" s="255" t="inlineStr">
         <is>
           <t>National Champion</t>
         </is>
@@ -20503,13 +20503,13 @@
         <f>_xlfn.XLOOKUP(AG31,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG31" s="257">
+      <c r="AG31" s="263">
         <f>Games!O49</f>
         <v/>
       </c>
       <c r="AH31" s="55" t="n"/>
       <c r="AI31" s="51" t="n"/>
-      <c r="AJ31" s="276">
+      <c r="AJ31" s="282">
         <f>IF($AU$5=TRUE,AJ23+1,"")</f>
         <v/>
       </c>
@@ -20530,11 +20530,11 @@
       </c>
     </row>
     <row r="32" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A32" s="278" t="n"/>
+      <c r="A32" s="286" t="n"/>
       <c r="B32" s="28" t="n"/>
       <c r="C32" s="38" t="n"/>
       <c r="D32" s="71" t="n"/>
-      <c r="G32" s="255" t="n"/>
+      <c r="G32" s="283" t="n"/>
       <c r="H32" s="50" t="n"/>
       <c r="I32" s="302" t="n"/>
       <c r="J32" s="307" t="n"/>
@@ -20563,10 +20563,10 @@
       <c r="AH32" s="56" t="n"/>
       <c r="AM32" s="39" t="n"/>
       <c r="AN32" s="28" t="n"/>
-      <c r="AO32" s="277" t="n"/>
+      <c r="AO32" s="287" t="n"/>
     </row>
     <row r="33" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A33" s="278" t="n"/>
+      <c r="A33" s="286" t="n"/>
       <c r="B33" s="27" t="n">
         <v>2</v>
       </c>
@@ -20582,11 +20582,11 @@
         <f>Games!L12</f>
         <v/>
       </c>
-      <c r="F33" s="257">
+      <c r="F33" s="263">
         <f>Games!O12</f>
         <v/>
       </c>
-      <c r="G33" s="260">
+      <c r="G33" s="248">
         <f>_xlfn.XLOOKUP(F33,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20594,8 +20594,8 @@
         <f>Games!N41</f>
         <v/>
       </c>
-      <c r="I33" s="286" t="n"/>
-      <c r="J33" s="286" t="n"/>
+      <c r="I33" s="255" t="n"/>
+      <c r="J33" s="255" t="n"/>
       <c r="L33" s="25" t="n"/>
       <c r="M33" s="25" t="n"/>
       <c r="O33" s="25" t="n"/>
@@ -20611,7 +20611,7 @@
       <c r="Y33" s="56" t="n"/>
       <c r="AA33" s="25" t="n"/>
       <c r="AD33" s="25" t="n"/>
-      <c r="AG33" s="286" t="n"/>
+      <c r="AG33" s="255" t="n"/>
       <c r="AH33" s="59">
         <f>Games!N49</f>
         <v/>
@@ -20620,7 +20620,7 @@
         <f>_xlfn.XLOOKUP(AJ33,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ33" s="257">
+      <c r="AJ33" s="263">
         <f>Games!O28</f>
         <v/>
       </c>
@@ -20639,11 +20639,11 @@
       <c r="AN33" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="AO33" s="277" t="n"/>
+      <c r="AO33" s="287" t="n"/>
       <c r="AQ33" s="9" t="n"/>
     </row>
     <row r="34" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A34" s="255">
+      <c r="A34" s="283">
         <f>IF($AU$5=TRUE,A30+1,"")</f>
         <v/>
       </c>
@@ -20654,8 +20654,8 @@
       <c r="F34" s="303" t="n"/>
       <c r="G34" s="307" t="n"/>
       <c r="H34" s="311" t="n"/>
-      <c r="I34" s="286" t="n"/>
-      <c r="J34" s="286" t="n"/>
+      <c r="I34" s="255" t="n"/>
+      <c r="J34" s="255" t="n"/>
       <c r="L34" s="25" t="n"/>
       <c r="M34" s="25" t="n"/>
       <c r="O34" s="25" t="n"/>
@@ -20671,18 +20671,18 @@
       <c r="Y34" s="56" t="n"/>
       <c r="AA34" s="25" t="n"/>
       <c r="AD34" s="25" t="n"/>
-      <c r="AG34" s="286" t="n"/>
+      <c r="AG34" s="255" t="n"/>
       <c r="AH34" s="312" t="n"/>
       <c r="AI34" s="303" t="n"/>
       <c r="AJ34" s="303" t="n"/>
       <c r="AK34" s="55" t="n"/>
       <c r="AM34" s="39" t="n"/>
       <c r="AN34" s="28" t="n"/>
-      <c r="AO34" s="277">
+      <c r="AO34" s="287">
         <f>IF($AU$5=TRUE,AO30+1,"")</f>
         <v/>
       </c>
-      <c r="AQ34" s="275" t="n"/>
+      <c r="AQ34" s="288" t="n"/>
     </row>
     <row r="35" ht="16.2" customHeight="1" thickBot="1">
       <c r="B35" s="27" t="n">
@@ -20700,10 +20700,10 @@
         <f>Games!N12</f>
         <v/>
       </c>
-      <c r="F35" s="286" t="n"/>
-      <c r="G35" s="286" t="n"/>
-      <c r="I35" s="286" t="n"/>
-      <c r="J35" s="286" t="n"/>
+      <c r="F35" s="255" t="n"/>
+      <c r="G35" s="255" t="n"/>
+      <c r="I35" s="255" t="n"/>
+      <c r="J35" s="255" t="n"/>
       <c r="L35" s="25" t="n"/>
       <c r="M35" s="25" t="n"/>
       <c r="O35" s="18">
@@ -20714,20 +20714,20 @@
       <c r="Q35" s="50" t="n"/>
       <c r="R35" s="25" t="n"/>
       <c r="S35" s="25" t="n"/>
-      <c r="T35" s="255">
+      <c r="T35" s="283">
         <f>IF($AU$5=TRUE,AA35+1,"")</f>
         <v/>
       </c>
       <c r="W35" s="25" t="n"/>
       <c r="X35" s="25" t="n"/>
       <c r="Y35" s="56" t="n"/>
-      <c r="AA35" s="278">
+      <c r="AA35" s="286">
         <f>IF($AU$5=TRUE,O35+1,"")</f>
         <v/>
       </c>
       <c r="AD35" s="25" t="n"/>
-      <c r="AG35" s="286" t="n"/>
-      <c r="AJ35" s="286" t="n"/>
+      <c r="AG35" s="255" t="n"/>
+      <c r="AJ35" s="255" t="n"/>
       <c r="AK35" s="59">
         <f>Games!N28</f>
         <v/>
@@ -20745,14 +20745,14 @@
       </c>
     </row>
     <row r="36" ht="10.5" customHeight="1">
-      <c r="A36" s="278" t="n"/>
+      <c r="A36" s="286" t="n"/>
       <c r="B36" s="28" t="n"/>
       <c r="C36" s="38" t="n"/>
       <c r="D36" s="71" t="n"/>
-      <c r="F36" s="286" t="n"/>
-      <c r="G36" s="286" t="n"/>
-      <c r="I36" s="286" t="n"/>
-      <c r="J36" s="286" t="n"/>
+      <c r="F36" s="255" t="n"/>
+      <c r="G36" s="255" t="n"/>
+      <c r="I36" s="255" t="n"/>
+      <c r="J36" s="255" t="n"/>
       <c r="L36" s="25" t="n"/>
       <c r="M36" s="25" t="n"/>
       <c r="O36" s="25" t="n"/>
@@ -20768,14 +20768,14 @@
       <c r="Y36" s="56" t="n"/>
       <c r="AA36" s="25" t="n"/>
       <c r="AD36" s="25" t="n"/>
-      <c r="AG36" s="286" t="n"/>
-      <c r="AJ36" s="286" t="n"/>
+      <c r="AG36" s="255" t="n"/>
+      <c r="AJ36" s="255" t="n"/>
       <c r="AM36" s="39" t="n"/>
       <c r="AN36" s="28" t="n"/>
-      <c r="AO36" s="277" t="n"/>
+      <c r="AO36" s="287" t="n"/>
     </row>
     <row r="37" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A37" s="278" t="n"/>
+      <c r="A37" s="286" t="n"/>
       <c r="B37" s="27" t="n">
         <v>1</v>
       </c>
@@ -20791,11 +20791,11 @@
         <f>Games!L13</f>
         <v/>
       </c>
-      <c r="F37" s="257">
+      <c r="F37" s="263">
         <f>Games!O13</f>
         <v/>
       </c>
-      <c r="G37" s="260">
+      <c r="G37" s="248">
         <f>_xlfn.XLOOKUP(F37,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20803,8 +20803,8 @@
         <f>Games!L42</f>
         <v/>
       </c>
-      <c r="I37" s="286" t="n"/>
-      <c r="J37" s="286" t="n"/>
+      <c r="I37" s="255" t="n"/>
+      <c r="J37" s="255" t="n"/>
       <c r="L37" s="25" t="n"/>
       <c r="M37" s="25" t="n"/>
       <c r="O37" s="25" t="n"/>
@@ -20820,7 +20820,7 @@
       <c r="Y37" s="56" t="n"/>
       <c r="AA37" s="25" t="n"/>
       <c r="AD37" s="25" t="n"/>
-      <c r="AG37" s="286" t="n"/>
+      <c r="AG37" s="255" t="n"/>
       <c r="AH37" s="58">
         <f>Games!L50</f>
         <v/>
@@ -20829,7 +20829,7 @@
         <f>_xlfn.XLOOKUP(AJ37,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ37" s="257">
+      <c r="AJ37" s="263">
         <f>Games!O29</f>
         <v/>
       </c>
@@ -20848,10 +20848,10 @@
       <c r="AN37" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="AO37" s="277" t="n"/>
+      <c r="AO37" s="287" t="n"/>
     </row>
     <row r="38" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A38" s="255">
+      <c r="A38" s="283">
         <f>IF($AU$5=TRUE,A34+1,"")</f>
         <v/>
       </c>
@@ -20862,8 +20862,8 @@
       <c r="F38" s="303" t="n"/>
       <c r="G38" s="307" t="n"/>
       <c r="H38" s="308" t="n"/>
-      <c r="I38" s="286" t="n"/>
-      <c r="J38" s="286" t="n"/>
+      <c r="I38" s="255" t="n"/>
+      <c r="J38" s="255" t="n"/>
       <c r="L38" s="25" t="n"/>
       <c r="M38" s="25" t="n"/>
       <c r="O38" s="25" t="n"/>
@@ -20879,14 +20879,14 @@
       <c r="Y38" s="56" t="n"/>
       <c r="AA38" s="25" t="n"/>
       <c r="AD38" s="25" t="n"/>
-      <c r="AG38" s="286" t="n"/>
+      <c r="AG38" s="255" t="n"/>
       <c r="AH38" s="308" t="n"/>
       <c r="AI38" s="303" t="n"/>
       <c r="AJ38" s="303" t="n"/>
       <c r="AK38" s="55" t="n"/>
       <c r="AM38" s="39" t="n"/>
       <c r="AN38" s="28" t="n"/>
-      <c r="AO38" s="277">
+      <c r="AO38" s="287">
         <f>IF($AU$5=TRUE,AO34+1,"")</f>
         <v/>
       </c>
@@ -20907,17 +20907,17 @@
         <f>Games!N13</f>
         <v/>
       </c>
-      <c r="F39" s="276">
+      <c r="F39" s="282">
         <f>IF($AU$5=TRUE,F31+1,"")</f>
         <v/>
       </c>
-      <c r="G39" s="276" t="n"/>
+      <c r="G39" s="282" t="n"/>
       <c r="H39" s="49" t="n"/>
-      <c r="I39" s="264">
+      <c r="I39" s="280">
         <f>Games!O42</f>
         <v/>
       </c>
-      <c r="J39" s="260">
+      <c r="J39" s="248">
         <f>_xlfn.XLOOKUP(I39,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -20936,11 +20936,11 @@
         <f>Games!N72</f>
         <v/>
       </c>
-      <c r="U39" s="266">
+      <c r="U39" s="294">
         <f>_xlfn.XLOOKUP(V39,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="V39" s="268">
+      <c r="V39" s="296">
         <f>Games!O70</f>
         <v/>
       </c>
@@ -20956,13 +20956,13 @@
         <f>_xlfn.XLOOKUP(AG39,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG39" s="257">
+      <c r="AG39" s="263">
         <f>Games!O50</f>
         <v/>
       </c>
       <c r="AH39" s="55" t="n"/>
       <c r="AI39" s="51" t="n"/>
-      <c r="AJ39" s="276">
+      <c r="AJ39" s="282">
         <f>IF($AU$5=TRUE,AJ31+1,"")</f>
         <v/>
       </c>
@@ -20983,11 +20983,11 @@
       </c>
     </row>
     <row r="40" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A40" s="278" t="n"/>
+      <c r="A40" s="286" t="n"/>
       <c r="B40" s="28" t="n"/>
       <c r="C40" s="38" t="n"/>
       <c r="D40" s="71" t="n"/>
-      <c r="G40" s="255" t="n"/>
+      <c r="G40" s="283" t="n"/>
       <c r="H40" s="50" t="n"/>
       <c r="I40" s="302" t="n"/>
       <c r="J40" s="307" t="n"/>
@@ -21013,10 +21013,10 @@
       <c r="AH40" s="56" t="n"/>
       <c r="AM40" s="39" t="n"/>
       <c r="AN40" s="28" t="n"/>
-      <c r="AO40" s="277" t="n"/>
+      <c r="AO40" s="287" t="n"/>
     </row>
     <row r="41" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A41" s="278" t="n"/>
+      <c r="A41" s="286" t="n"/>
       <c r="B41" s="27" t="n">
         <v>8</v>
       </c>
@@ -21032,11 +21032,11 @@
         <f>Games!L14</f>
         <v/>
       </c>
-      <c r="F41" s="257">
+      <c r="F41" s="263">
         <f>Games!O14</f>
         <v/>
       </c>
-      <c r="G41" s="260">
+      <c r="G41" s="248">
         <f>_xlfn.XLOOKUP(F41,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21044,8 +21044,8 @@
         <f>Games!N42</f>
         <v/>
       </c>
-      <c r="I41" s="286" t="n"/>
-      <c r="J41" s="286" t="n"/>
+      <c r="I41" s="255" t="n"/>
+      <c r="J41" s="255" t="n"/>
       <c r="K41" s="49" t="n"/>
       <c r="L41" s="25" t="n"/>
       <c r="M41" s="25" t="n"/>
@@ -21063,7 +21063,7 @@
       <c r="AA41" s="25" t="n"/>
       <c r="AD41" s="25" t="n"/>
       <c r="AE41" s="55" t="n"/>
-      <c r="AG41" s="286" t="n"/>
+      <c r="AG41" s="255" t="n"/>
       <c r="AH41" s="59">
         <f>Games!N50</f>
         <v/>
@@ -21072,7 +21072,7 @@
         <f>_xlfn.XLOOKUP(AJ41,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ41" s="257">
+      <c r="AJ41" s="263">
         <f>Games!O30</f>
         <v/>
       </c>
@@ -21091,10 +21091,10 @@
       <c r="AN41" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="AO41" s="277" t="n"/>
+      <c r="AO41" s="287" t="n"/>
     </row>
     <row r="42" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A42" s="255">
+      <c r="A42" s="283">
         <f>IF($AU$5=TRUE,A38+1,"")</f>
         <v/>
       </c>
@@ -21105,8 +21105,8 @@
       <c r="F42" s="303" t="n"/>
       <c r="G42" s="307" t="n"/>
       <c r="H42" s="311" t="n"/>
-      <c r="I42" s="286" t="n"/>
-      <c r="J42" s="286" t="n"/>
+      <c r="I42" s="255" t="n"/>
+      <c r="J42" s="255" t="n"/>
       <c r="K42" s="50" t="n"/>
       <c r="L42" s="25" t="n"/>
       <c r="M42" s="25" t="n"/>
@@ -21124,14 +21124,14 @@
       <c r="AA42" s="25" t="n"/>
       <c r="AD42" s="25" t="n"/>
       <c r="AE42" s="56" t="n"/>
-      <c r="AG42" s="286" t="n"/>
+      <c r="AG42" s="255" t="n"/>
       <c r="AH42" s="312" t="n"/>
       <c r="AI42" s="303" t="n"/>
       <c r="AJ42" s="303" t="n"/>
       <c r="AK42" s="55" t="n"/>
       <c r="AM42" s="39" t="n"/>
       <c r="AN42" s="28" t="n"/>
-      <c r="AO42" s="277">
+      <c r="AO42" s="287">
         <f>IF($AU$5=TRUE,AO38+1,"")</f>
         <v/>
       </c>
@@ -21152,19 +21152,19 @@
         <f>Games!N14</f>
         <v/>
       </c>
-      <c r="F43" s="286" t="n"/>
-      <c r="G43" s="286" t="n"/>
-      <c r="I43" s="255">
+      <c r="F43" s="255" t="n"/>
+      <c r="G43" s="255" t="n"/>
+      <c r="I43" s="283">
         <f>IF($AU$5=TRUE,I27+1,"")</f>
         <v/>
       </c>
-      <c r="J43" s="255" t="n"/>
+      <c r="J43" s="283" t="n"/>
       <c r="K43" s="50" t="n"/>
-      <c r="L43" s="264">
+      <c r="L43" s="280">
         <f>Games!O57</f>
         <v/>
       </c>
-      <c r="M43" s="260">
+      <c r="M43" s="248">
         <f>_xlfn.XLOOKUP(L43,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21192,16 +21192,16 @@
         <f>_xlfn.XLOOKUP(AD43,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AD43" s="262">
+      <c r="AD43" s="292">
         <f>Games!O61</f>
         <v/>
       </c>
       <c r="AE43" s="56" t="n"/>
-      <c r="AG43" s="255">
+      <c r="AG43" s="283">
         <f>IF($AU$5=TRUE,AG27+1,"")</f>
         <v/>
       </c>
-      <c r="AJ43" s="286" t="n"/>
+      <c r="AJ43" s="255" t="n"/>
       <c r="AK43" s="59">
         <f>Games!N30</f>
         <v/>
@@ -21219,13 +21219,13 @@
       </c>
     </row>
     <row r="44" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A44" s="278" t="n"/>
+      <c r="A44" s="286" t="n"/>
       <c r="B44" s="28" t="n"/>
       <c r="C44" s="38" t="n"/>
       <c r="D44" s="71" t="n"/>
-      <c r="F44" s="286" t="n"/>
-      <c r="G44" s="286" t="n"/>
-      <c r="J44" s="255" t="n"/>
+      <c r="F44" s="255" t="n"/>
+      <c r="G44" s="255" t="n"/>
+      <c r="J44" s="283" t="n"/>
       <c r="K44" s="50" t="n"/>
       <c r="L44" s="302" t="n"/>
       <c r="M44" s="307" t="n"/>
@@ -21246,13 +21246,13 @@
       <c r="AC44" s="303" t="n"/>
       <c r="AD44" s="303" t="n"/>
       <c r="AE44" s="56" t="n"/>
-      <c r="AJ44" s="286" t="n"/>
+      <c r="AJ44" s="255" t="n"/>
       <c r="AM44" s="39" t="n"/>
       <c r="AN44" s="28" t="n"/>
-      <c r="AO44" s="277" t="n"/>
+      <c r="AO44" s="287" t="n"/>
     </row>
     <row r="45" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A45" s="278" t="n"/>
+      <c r="A45" s="286" t="n"/>
       <c r="B45" s="27" t="n">
         <v>5</v>
       </c>
@@ -21268,11 +21268,11 @@
         <f>Games!L15</f>
         <v/>
       </c>
-      <c r="F45" s="257">
+      <c r="F45" s="263">
         <f>Games!O15</f>
         <v/>
       </c>
-      <c r="G45" s="260">
+      <c r="G45" s="248">
         <f>_xlfn.XLOOKUP(F45,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21280,8 +21280,8 @@
         <f>Games!L43</f>
         <v/>
       </c>
-      <c r="I45" s="286" t="n"/>
-      <c r="J45" s="286" t="n"/>
+      <c r="I45" s="255" t="n"/>
+      <c r="J45" s="255" t="n"/>
       <c r="K45" s="50" t="n"/>
       <c r="L45" s="25" t="n"/>
       <c r="M45" s="25" t="n"/>
@@ -21301,7 +21301,7 @@
       <c r="AB45" s="55" t="n"/>
       <c r="AD45" s="25" t="n"/>
       <c r="AE45" s="56" t="n"/>
-      <c r="AG45" s="286" t="n"/>
+      <c r="AG45" s="255" t="n"/>
       <c r="AH45" s="58">
         <f>Games!L51</f>
         <v/>
@@ -21310,7 +21310,7 @@
         <f>_xlfn.XLOOKUP(AJ45,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ45" s="257">
+      <c r="AJ45" s="263">
         <f>Games!O31</f>
         <v/>
       </c>
@@ -21329,10 +21329,10 @@
       <c r="AN45" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="AO45" s="277" t="n"/>
+      <c r="AO45" s="287" t="n"/>
     </row>
     <row r="46" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A46" s="255">
+      <c r="A46" s="283">
         <f>IF($AU$5=TRUE,A42+1,"")</f>
         <v/>
       </c>
@@ -21343,8 +21343,8 @@
       <c r="F46" s="303" t="n"/>
       <c r="G46" s="307" t="n"/>
       <c r="H46" s="308" t="n"/>
-      <c r="I46" s="286" t="n"/>
-      <c r="J46" s="286" t="n"/>
+      <c r="I46" s="255" t="n"/>
+      <c r="J46" s="255" t="n"/>
       <c r="K46" s="50" t="n"/>
       <c r="L46" s="25" t="n"/>
       <c r="M46" s="25" t="n"/>
@@ -21364,14 +21364,14 @@
       <c r="AB46" s="56" t="n"/>
       <c r="AD46" s="25" t="n"/>
       <c r="AE46" s="56" t="n"/>
-      <c r="AG46" s="286" t="n"/>
+      <c r="AG46" s="255" t="n"/>
       <c r="AH46" s="308" t="n"/>
       <c r="AI46" s="303" t="n"/>
       <c r="AJ46" s="303" t="n"/>
       <c r="AK46" s="55" t="n"/>
       <c r="AM46" s="39" t="n"/>
       <c r="AN46" s="28" t="n"/>
-      <c r="AO46" s="277">
+      <c r="AO46" s="287">
         <f>IF($AU$5=TRUE,AO42+1,"")</f>
         <v/>
       </c>
@@ -21392,17 +21392,17 @@
         <f>Games!N15</f>
         <v/>
       </c>
-      <c r="F47" s="276">
+      <c r="F47" s="282">
         <f>IF($AU$5=TRUE,F39+1,"")</f>
         <v/>
       </c>
-      <c r="G47" s="276" t="n"/>
+      <c r="G47" s="282" t="n"/>
       <c r="H47" s="49" t="n"/>
-      <c r="I47" s="264">
+      <c r="I47" s="280">
         <f>Games!O43</f>
         <v/>
       </c>
-      <c r="J47" s="260">
+      <c r="J47" s="248">
         <f>_xlfn.XLOOKUP(I47,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21435,13 +21435,13 @@
         <f>_xlfn.XLOOKUP(AG47,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG47" s="257">
+      <c r="AG47" s="263">
         <f>Games!O51</f>
         <v/>
       </c>
       <c r="AH47" s="55" t="n"/>
       <c r="AI47" s="51" t="n"/>
-      <c r="AJ47" s="276">
+      <c r="AJ47" s="282">
         <f>IF($AU$5=TRUE,AJ39+1,"")</f>
         <v/>
       </c>
@@ -21462,11 +21462,11 @@
       </c>
     </row>
     <row r="48" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A48" s="278" t="n"/>
+      <c r="A48" s="286" t="n"/>
       <c r="B48" s="28" t="n"/>
       <c r="C48" s="38" t="n"/>
       <c r="D48" s="71" t="n"/>
-      <c r="G48" s="255" t="n"/>
+      <c r="G48" s="283" t="n"/>
       <c r="H48" s="50" t="n"/>
       <c r="I48" s="302" t="n"/>
       <c r="J48" s="307" t="n"/>
@@ -21494,10 +21494,10 @@
       <c r="AH48" s="56" t="n"/>
       <c r="AM48" s="39" t="n"/>
       <c r="AN48" s="28" t="n"/>
-      <c r="AO48" s="277" t="n"/>
+      <c r="AO48" s="287" t="n"/>
     </row>
     <row r="49" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A49" s="278" t="n"/>
+      <c r="A49" s="286" t="n"/>
       <c r="B49" s="27" t="n">
         <v>4</v>
       </c>
@@ -21513,11 +21513,11 @@
         <f>Games!L16</f>
         <v/>
       </c>
-      <c r="F49" s="257">
+      <c r="F49" s="263">
         <f>Games!O16</f>
         <v/>
       </c>
-      <c r="G49" s="260">
+      <c r="G49" s="248">
         <f>_xlfn.XLOOKUP(F49,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21525,8 +21525,8 @@
         <f>Games!N43</f>
         <v/>
       </c>
-      <c r="I49" s="286" t="n"/>
-      <c r="J49" s="286" t="n"/>
+      <c r="I49" s="255" t="n"/>
+      <c r="J49" s="255" t="n"/>
       <c r="L49" s="25" t="n"/>
       <c r="M49" s="25" t="n"/>
       <c r="N49" s="50" t="n"/>
@@ -21544,7 +21544,7 @@
       <c r="AA49" s="25" t="n"/>
       <c r="AB49" s="56" t="n"/>
       <c r="AD49" s="25" t="n"/>
-      <c r="AG49" s="286" t="n"/>
+      <c r="AG49" s="255" t="n"/>
       <c r="AH49" s="59">
         <f>Games!N51</f>
         <v/>
@@ -21553,7 +21553,7 @@
         <f>_xlfn.XLOOKUP(AJ49,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ49" s="257">
+      <c r="AJ49" s="263">
         <f>Games!O32</f>
         <v/>
       </c>
@@ -21572,10 +21572,10 @@
       <c r="AN49" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="AO49" s="277" t="n"/>
+      <c r="AO49" s="287" t="n"/>
     </row>
     <row r="50" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A50" s="255">
+      <c r="A50" s="283">
         <f>IF($AU$5=TRUE,A46+1,"")</f>
         <v/>
       </c>
@@ -21586,8 +21586,8 @@
       <c r="F50" s="303" t="n"/>
       <c r="G50" s="307" t="n"/>
       <c r="H50" s="311" t="n"/>
-      <c r="I50" s="286" t="n"/>
-      <c r="J50" s="286" t="n"/>
+      <c r="I50" s="255" t="n"/>
+      <c r="J50" s="255" t="n"/>
       <c r="L50" s="25" t="n"/>
       <c r="M50" s="25" t="n"/>
       <c r="N50" s="50" t="n"/>
@@ -21605,14 +21605,14 @@
       <c r="AA50" s="25" t="n"/>
       <c r="AB50" s="56" t="n"/>
       <c r="AD50" s="25" t="n"/>
-      <c r="AG50" s="286" t="n"/>
+      <c r="AG50" s="255" t="n"/>
       <c r="AH50" s="312" t="n"/>
       <c r="AI50" s="303" t="n"/>
       <c r="AJ50" s="303" t="n"/>
       <c r="AK50" s="55" t="n"/>
       <c r="AM50" s="39" t="n"/>
       <c r="AN50" s="28" t="n"/>
-      <c r="AO50" s="277">
+      <c r="AO50" s="287">
         <f>IF($AU$5=TRUE,AO46+1,"")</f>
         <v/>
       </c>
@@ -21633,22 +21633,22 @@
         <f>Games!N16</f>
         <v/>
       </c>
-      <c r="F51" s="286" t="n"/>
-      <c r="G51" s="286" t="n"/>
-      <c r="I51" s="286" t="n"/>
-      <c r="J51" s="286" t="n"/>
-      <c r="K51" s="258" t="inlineStr">
+      <c r="F51" s="255" t="n"/>
+      <c r="G51" s="255" t="n"/>
+      <c r="I51" s="255" t="n"/>
+      <c r="J51" s="255" t="n"/>
+      <c r="K51" s="266" t="inlineStr">
         <is>
           <t>West</t>
         </is>
       </c>
-      <c r="M51" s="258" t="n"/>
+      <c r="M51" s="266" t="n"/>
       <c r="N51" s="50" t="n"/>
-      <c r="O51" s="264">
+      <c r="O51" s="280">
         <f>Games!O65</f>
         <v/>
       </c>
-      <c r="P51" s="260">
+      <c r="P51" s="248">
         <f>_xlfn.XLOOKUP(O51,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21671,19 +21671,19 @@
         <f>_xlfn.XLOOKUP(AA51,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AA51" s="257">
+      <c r="AA51" s="263">
         <f>Games!O67</f>
         <v/>
       </c>
       <c r="AB51" s="56" t="n"/>
-      <c r="AD51" s="258" t="inlineStr">
+      <c r="AD51" s="266" t="inlineStr">
         <is>
           <t>Midwest</t>
         </is>
       </c>
-      <c r="AF51" s="258" t="n"/>
-      <c r="AG51" s="286" t="n"/>
-      <c r="AJ51" s="286" t="n"/>
+      <c r="AF51" s="266" t="n"/>
+      <c r="AG51" s="255" t="n"/>
+      <c r="AJ51" s="255" t="n"/>
       <c r="AK51" s="59">
         <f>Games!N32</f>
         <v/>
@@ -21701,15 +21701,15 @@
       </c>
     </row>
     <row r="52" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A52" s="278" t="n"/>
+      <c r="A52" s="286" t="n"/>
       <c r="B52" s="28" t="n"/>
       <c r="C52" s="38" t="n"/>
       <c r="D52" s="71" t="n"/>
-      <c r="F52" s="286" t="n"/>
-      <c r="G52" s="286" t="n"/>
-      <c r="I52" s="286" t="n"/>
-      <c r="J52" s="286" t="n"/>
-      <c r="M52" s="258" t="n"/>
+      <c r="F52" s="255" t="n"/>
+      <c r="G52" s="255" t="n"/>
+      <c r="I52" s="255" t="n"/>
+      <c r="J52" s="255" t="n"/>
+      <c r="M52" s="266" t="n"/>
       <c r="N52" s="50" t="n"/>
       <c r="O52" s="302" t="n"/>
       <c r="P52" s="307" t="n"/>
@@ -21725,15 +21725,15 @@
       <c r="Z52" s="303" t="n"/>
       <c r="AA52" s="303" t="n"/>
       <c r="AB52" s="56" t="n"/>
-      <c r="AF52" s="258" t="n"/>
-      <c r="AG52" s="286" t="n"/>
-      <c r="AJ52" s="286" t="n"/>
+      <c r="AF52" s="266" t="n"/>
+      <c r="AG52" s="255" t="n"/>
+      <c r="AJ52" s="255" t="n"/>
       <c r="AM52" s="39" t="n"/>
       <c r="AN52" s="28" t="n"/>
-      <c r="AO52" s="277" t="n"/>
+      <c r="AO52" s="287" t="n"/>
     </row>
     <row r="53" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A53" s="278" t="n"/>
+      <c r="A53" s="286" t="n"/>
       <c r="B53" s="27" t="n">
         <v>6</v>
       </c>
@@ -21749,11 +21749,11 @@
         <f>Games!L17</f>
         <v/>
       </c>
-      <c r="F53" s="257">
+      <c r="F53" s="263">
         <f>Games!O17</f>
         <v/>
       </c>
-      <c r="G53" s="260">
+      <c r="G53" s="248">
         <f>_xlfn.XLOOKUP(F53,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21761,8 +21761,8 @@
         <f>Games!L44</f>
         <v/>
       </c>
-      <c r="I53" s="286" t="n"/>
-      <c r="J53" s="286" t="n"/>
+      <c r="I53" s="255" t="n"/>
+      <c r="J53" s="255" t="n"/>
       <c r="L53" s="18">
         <f>IF($AU$5=TRUE,L21+1,"")</f>
         <v/>
@@ -21781,11 +21781,11 @@
       <c r="X53" s="25" t="n"/>
       <c r="AA53" s="25" t="n"/>
       <c r="AB53" s="56" t="n"/>
-      <c r="AD53" s="278">
+      <c r="AD53" s="286">
         <f>IF($AU$5=TRUE,AD21+1,"")</f>
         <v/>
       </c>
-      <c r="AG53" s="286" t="n"/>
+      <c r="AG53" s="255" t="n"/>
       <c r="AH53" s="58">
         <f>Games!L52</f>
         <v/>
@@ -21794,7 +21794,7 @@
         <f>_xlfn.XLOOKUP(AJ53,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ53" s="257">
+      <c r="AJ53" s="263">
         <f>Games!O33</f>
         <v/>
       </c>
@@ -21813,10 +21813,10 @@
       <c r="AN53" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="AO53" s="277" t="n"/>
+      <c r="AO53" s="287" t="n"/>
     </row>
     <row r="54" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A54" s="255">
+      <c r="A54" s="283">
         <f>IF($AU$5=TRUE,A50+1,"")</f>
         <v/>
       </c>
@@ -21827,8 +21827,8 @@
       <c r="F54" s="303" t="n"/>
       <c r="G54" s="307" t="n"/>
       <c r="H54" s="308" t="n"/>
-      <c r="I54" s="286" t="n"/>
-      <c r="J54" s="286" t="n"/>
+      <c r="I54" s="255" t="n"/>
+      <c r="J54" s="255" t="n"/>
       <c r="L54" s="25" t="n"/>
       <c r="M54" s="25" t="n"/>
       <c r="N54" s="50" t="n"/>
@@ -21844,14 +21844,14 @@
       <c r="AA54" s="25" t="n"/>
       <c r="AB54" s="56" t="n"/>
       <c r="AD54" s="25" t="n"/>
-      <c r="AG54" s="286" t="n"/>
+      <c r="AG54" s="255" t="n"/>
       <c r="AH54" s="308" t="n"/>
       <c r="AI54" s="303" t="n"/>
       <c r="AJ54" s="303" t="n"/>
       <c r="AK54" s="55" t="n"/>
       <c r="AM54" s="39" t="n"/>
       <c r="AN54" s="28" t="n"/>
-      <c r="AO54" s="277">
+      <c r="AO54" s="287">
         <f>IF($AU$5=TRUE,AO50+1,"")</f>
         <v/>
       </c>
@@ -21872,17 +21872,17 @@
         <f>Games!N17</f>
         <v/>
       </c>
-      <c r="F55" s="276">
+      <c r="F55" s="282">
         <f>IF($AU$5=TRUE,F47+1,"")</f>
         <v/>
       </c>
-      <c r="G55" s="276" t="n"/>
+      <c r="G55" s="282" t="n"/>
       <c r="H55" s="49" t="n"/>
-      <c r="I55" s="264">
+      <c r="I55" s="280">
         <f>Games!O44</f>
         <v/>
       </c>
-      <c r="J55" s="260">
+      <c r="J55" s="248">
         <f>_xlfn.XLOOKUP(I55,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -21913,13 +21913,13 @@
         <f>_xlfn.XLOOKUP(AG55,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG55" s="257">
+      <c r="AG55" s="263">
         <f>Games!O52</f>
         <v/>
       </c>
       <c r="AH55" s="55" t="n"/>
       <c r="AI55" s="51" t="n"/>
-      <c r="AJ55" s="276">
+      <c r="AJ55" s="282">
         <f>IF($AU$5=TRUE,AJ47+1,"")</f>
         <v/>
       </c>
@@ -21940,11 +21940,11 @@
       </c>
     </row>
     <row r="56" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A56" s="278" t="n"/>
+      <c r="A56" s="286" t="n"/>
       <c r="B56" s="28" t="n"/>
       <c r="C56" s="38" t="n"/>
       <c r="D56" s="71" t="n"/>
-      <c r="G56" s="255" t="n"/>
+      <c r="G56" s="283" t="n"/>
       <c r="H56" s="50" t="n"/>
       <c r="I56" s="302" t="n"/>
       <c r="J56" s="307" t="n"/>
@@ -21970,10 +21970,10 @@
       <c r="AH56" s="56" t="n"/>
       <c r="AM56" s="39" t="n"/>
       <c r="AN56" s="28" t="n"/>
-      <c r="AO56" s="277" t="n"/>
+      <c r="AO56" s="287" t="n"/>
     </row>
     <row r="57" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A57" s="278" t="n"/>
+      <c r="A57" s="286" t="n"/>
       <c r="B57" s="27" t="n">
         <v>3</v>
       </c>
@@ -21989,11 +21989,11 @@
         <f>Games!L18</f>
         <v/>
       </c>
-      <c r="F57" s="257">
+      <c r="F57" s="263">
         <f>Games!O18</f>
         <v/>
       </c>
-      <c r="G57" s="260">
+      <c r="G57" s="248">
         <f>_xlfn.XLOOKUP(F57,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -22001,8 +22001,8 @@
         <f>Games!N44</f>
         <v/>
       </c>
-      <c r="I57" s="286" t="n"/>
-      <c r="J57" s="286" t="n"/>
+      <c r="I57" s="255" t="n"/>
+      <c r="J57" s="255" t="n"/>
       <c r="K57" s="49" t="n"/>
       <c r="L57" s="25" t="n"/>
       <c r="M57" s="25" t="n"/>
@@ -22020,7 +22020,7 @@
       <c r="AB57" s="56" t="n"/>
       <c r="AD57" s="25" t="n"/>
       <c r="AE57" s="55" t="n"/>
-      <c r="AG57" s="286" t="n"/>
+      <c r="AG57" s="255" t="n"/>
       <c r="AH57" s="59">
         <f>Games!N52</f>
         <v/>
@@ -22029,7 +22029,7 @@
         <f>_xlfn.XLOOKUP(AJ57,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ57" s="257">
+      <c r="AJ57" s="263">
         <f>Games!O34</f>
         <v/>
       </c>
@@ -22048,10 +22048,10 @@
       <c r="AN57" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="AO57" s="277" t="n"/>
+      <c r="AO57" s="287" t="n"/>
     </row>
     <row r="58" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A58" s="255">
+      <c r="A58" s="283">
         <f>IF($AU$5=TRUE,A54+1,"")</f>
         <v/>
       </c>
@@ -22062,8 +22062,8 @@
       <c r="F58" s="303" t="n"/>
       <c r="G58" s="307" t="n"/>
       <c r="H58" s="311" t="n"/>
-      <c r="I58" s="286" t="n"/>
-      <c r="J58" s="286" t="n"/>
+      <c r="I58" s="255" t="n"/>
+      <c r="J58" s="255" t="n"/>
       <c r="K58" s="50" t="n"/>
       <c r="L58" s="25" t="n"/>
       <c r="M58" s="25" t="n"/>
@@ -22081,14 +22081,14 @@
       <c r="AB58" s="56" t="n"/>
       <c r="AD58" s="25" t="n"/>
       <c r="AE58" s="56" t="n"/>
-      <c r="AG58" s="286" t="n"/>
+      <c r="AG58" s="255" t="n"/>
       <c r="AH58" s="312" t="n"/>
       <c r="AI58" s="303" t="n"/>
       <c r="AJ58" s="303" t="n"/>
       <c r="AK58" s="55" t="n"/>
       <c r="AM58" s="39" t="n"/>
       <c r="AN58" s="28" t="n"/>
-      <c r="AO58" s="277">
+      <c r="AO58" s="287">
         <f>IF($AU$5=TRUE,AO54+1,"")</f>
         <v/>
       </c>
@@ -22109,19 +22109,19 @@
         <f>Games!N18</f>
         <v/>
       </c>
-      <c r="F59" s="286" t="n"/>
-      <c r="G59" s="286" t="n"/>
-      <c r="I59" s="255">
+      <c r="F59" s="255" t="n"/>
+      <c r="G59" s="255" t="n"/>
+      <c r="I59" s="283">
         <f>IF($AU$5=TRUE,I43+1,"")</f>
         <v/>
       </c>
-      <c r="J59" s="255" t="n"/>
+      <c r="J59" s="283" t="n"/>
       <c r="K59" s="50" t="n"/>
-      <c r="L59" s="264">
+      <c r="L59" s="280">
         <f>Games!O58</f>
         <v/>
       </c>
-      <c r="M59" s="260">
+      <c r="M59" s="248">
         <f>_xlfn.XLOOKUP(L59,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -22147,16 +22147,16 @@
         <f>_xlfn.XLOOKUP(AD59,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AD59" s="257">
+      <c r="AD59" s="263">
         <f>Games!O62</f>
         <v/>
       </c>
       <c r="AE59" s="56" t="n"/>
-      <c r="AG59" s="255">
+      <c r="AG59" s="283">
         <f>IF($AU$5=TRUE,AG43+1,"")</f>
         <v/>
       </c>
-      <c r="AJ59" s="286" t="n"/>
+      <c r="AJ59" s="255" t="n"/>
       <c r="AK59" s="59">
         <f>Games!N34</f>
         <v/>
@@ -22174,13 +22174,13 @@
       </c>
     </row>
     <row r="60" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A60" s="278" t="n"/>
+      <c r="A60" s="286" t="n"/>
       <c r="B60" s="28" t="n"/>
       <c r="C60" s="38" t="n"/>
       <c r="D60" s="71" t="n"/>
-      <c r="F60" s="286" t="n"/>
-      <c r="G60" s="286" t="n"/>
-      <c r="J60" s="255" t="n"/>
+      <c r="F60" s="255" t="n"/>
+      <c r="G60" s="255" t="n"/>
+      <c r="J60" s="283" t="n"/>
       <c r="K60" s="50" t="n"/>
       <c r="L60" s="302" t="n"/>
       <c r="M60" s="307" t="n"/>
@@ -22200,13 +22200,13 @@
       <c r="AC60" s="303" t="n"/>
       <c r="AD60" s="303" t="n"/>
       <c r="AE60" s="56" t="n"/>
-      <c r="AJ60" s="286" t="n"/>
+      <c r="AJ60" s="255" t="n"/>
       <c r="AM60" s="39" t="n"/>
       <c r="AN60" s="28" t="n"/>
-      <c r="AO60" s="277" t="n"/>
+      <c r="AO60" s="287" t="n"/>
     </row>
     <row r="61" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A61" s="278" t="n"/>
+      <c r="A61" s="286" t="n"/>
       <c r="B61" s="27" t="n">
         <v>7</v>
       </c>
@@ -22222,11 +22222,11 @@
         <f>Games!L19</f>
         <v/>
       </c>
-      <c r="F61" s="257">
+      <c r="F61" s="263">
         <f>Games!O19</f>
         <v/>
       </c>
-      <c r="G61" s="260">
+      <c r="G61" s="248">
         <f>_xlfn.XLOOKUP(F61,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -22234,8 +22234,8 @@
         <f>Games!L45</f>
         <v/>
       </c>
-      <c r="I61" s="286" t="n"/>
-      <c r="J61" s="286" t="n"/>
+      <c r="I61" s="255" t="n"/>
+      <c r="J61" s="255" t="n"/>
       <c r="K61" s="50" t="n"/>
       <c r="L61" s="25" t="n"/>
       <c r="M61" s="25" t="n"/>
@@ -22252,7 +22252,7 @@
       <c r="AA61" s="25" t="n"/>
       <c r="AD61" s="25" t="n"/>
       <c r="AE61" s="56" t="n"/>
-      <c r="AG61" s="286" t="n"/>
+      <c r="AG61" s="255" t="n"/>
       <c r="AH61" s="58">
         <f>Games!L53</f>
         <v/>
@@ -22261,7 +22261,7 @@
         <f>_xlfn.XLOOKUP(AJ61,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ61" s="257">
+      <c r="AJ61" s="263">
         <f>Games!O35</f>
         <v/>
       </c>
@@ -22280,10 +22280,10 @@
       <c r="AN61" s="27" t="n">
         <v>7</v>
       </c>
-      <c r="AO61" s="277" t="n"/>
+      <c r="AO61" s="287" t="n"/>
     </row>
     <row r="62" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A62" s="255">
+      <c r="A62" s="283">
         <f>IF($AU$5=TRUE,A58+1,"")</f>
         <v/>
       </c>
@@ -22294,8 +22294,8 @@
       <c r="F62" s="303" t="n"/>
       <c r="G62" s="307" t="n"/>
       <c r="H62" s="308" t="n"/>
-      <c r="I62" s="286" t="n"/>
-      <c r="J62" s="286" t="n"/>
+      <c r="I62" s="255" t="n"/>
+      <c r="J62" s="255" t="n"/>
       <c r="K62" s="50" t="n"/>
       <c r="L62" s="25" t="n"/>
       <c r="M62" s="25" t="n"/>
@@ -22312,14 +22312,14 @@
       <c r="AA62" s="25" t="n"/>
       <c r="AD62" s="25" t="n"/>
       <c r="AE62" s="56" t="n"/>
-      <c r="AG62" s="286" t="n"/>
+      <c r="AG62" s="255" t="n"/>
       <c r="AH62" s="308" t="n"/>
       <c r="AI62" s="303" t="n"/>
       <c r="AJ62" s="303" t="n"/>
       <c r="AK62" s="55" t="n"/>
       <c r="AM62" s="39" t="n"/>
       <c r="AN62" s="28" t="n"/>
-      <c r="AO62" s="277">
+      <c r="AO62" s="287">
         <f>IF($AU$5=TRUE,AO58+1,"")</f>
         <v/>
       </c>
@@ -22340,17 +22340,17 @@
         <f>Games!N19</f>
         <v/>
       </c>
-      <c r="F63" s="276">
+      <c r="F63" s="282">
         <f>IF($AU$5=TRUE,F55+1,"")</f>
         <v/>
       </c>
-      <c r="G63" s="276" t="n"/>
+      <c r="G63" s="282" t="n"/>
       <c r="H63" s="49" t="n"/>
-      <c r="I63" s="264">
+      <c r="I63" s="280">
         <f>Games!O45</f>
         <v/>
       </c>
-      <c r="J63" s="260">
+      <c r="J63" s="248">
         <f>_xlfn.XLOOKUP(I63,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -22382,13 +22382,13 @@
         <f>_xlfn.XLOOKUP(AG63,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AG63" s="257">
+      <c r="AG63" s="263">
         <f>Games!O53</f>
         <v/>
       </c>
       <c r="AH63" s="55" t="n"/>
       <c r="AI63" s="51" t="n"/>
-      <c r="AJ63" s="276">
+      <c r="AJ63" s="282">
         <f>IF($AU$5=TRUE,AJ55+1,"")</f>
         <v/>
       </c>
@@ -22409,11 +22409,11 @@
       </c>
     </row>
     <row r="64" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A64" s="278" t="n"/>
+      <c r="A64" s="286" t="n"/>
       <c r="B64" s="28" t="n"/>
       <c r="C64" s="38" t="n"/>
       <c r="D64" s="71" t="n"/>
-      <c r="G64" s="255" t="n"/>
+      <c r="G64" s="283" t="n"/>
       <c r="H64" s="50" t="n"/>
       <c r="I64" s="302" t="n"/>
       <c r="J64" s="307" t="n"/>
@@ -22439,10 +22439,10 @@
       <c r="AH64" s="56" t="n"/>
       <c r="AM64" s="39" t="n"/>
       <c r="AN64" s="28" t="n"/>
-      <c r="AO64" s="277" t="n"/>
+      <c r="AO64" s="287" t="n"/>
     </row>
     <row r="65" ht="18.6" customHeight="1" thickBot="1">
-      <c r="A65" s="278" t="n"/>
+      <c r="A65" s="286" t="n"/>
       <c r="B65" s="27" t="n">
         <v>2</v>
       </c>
@@ -22458,11 +22458,11 @@
         <f>Games!L20</f>
         <v/>
       </c>
-      <c r="F65" s="257">
+      <c r="F65" s="263">
         <f>Games!O20</f>
         <v/>
       </c>
-      <c r="G65" s="260">
+      <c r="G65" s="248">
         <f>_xlfn.XLOOKUP(F65,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
@@ -22487,7 +22487,7 @@
       <c r="Z65" s="57" t="n"/>
       <c r="AA65" s="25" t="n"/>
       <c r="AD65" s="25" t="n"/>
-      <c r="AG65" s="286" t="n"/>
+      <c r="AG65" s="255" t="n"/>
       <c r="AH65" s="59">
         <f>Games!N53</f>
         <v/>
@@ -22496,7 +22496,7 @@
         <f>_xlfn.XLOOKUP(AJ65,Teams!$C:$C,Teams!$E:$E,,0,1)</f>
         <v/>
       </c>
-      <c r="AJ65" s="257">
+      <c r="AJ65" s="263">
         <f>Games!O36</f>
         <v/>
       </c>
@@ -22515,10 +22515,10 @@
       <c r="AN65" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="AO65" s="277" t="n"/>
+      <c r="AO65" s="287" t="n"/>
     </row>
     <row r="66" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A66" s="255">
+      <c r="A66" s="283">
         <f>IF($AU$5=TRUE,A62+1,"")</f>
         <v/>
       </c>
@@ -22533,16 +22533,16 @@
       <c r="J66" s="25" t="n"/>
       <c r="L66" s="25" t="n"/>
       <c r="M66" s="25" t="n"/>
-      <c r="O66" s="292" t="n"/>
+      <c r="O66" s="261" t="n"/>
       <c r="AD66" s="25" t="n"/>
-      <c r="AG66" s="286" t="n"/>
+      <c r="AG66" s="255" t="n"/>
       <c r="AH66" s="312" t="n"/>
       <c r="AI66" s="303" t="n"/>
       <c r="AJ66" s="303" t="n"/>
       <c r="AK66" s="55" t="n"/>
       <c r="AM66" s="39" t="n"/>
       <c r="AN66" s="28" t="n"/>
-      <c r="AO66" s="277">
+      <c r="AO66" s="287">
         <f>IF($AU$5=TRUE,AO62+1,"")</f>
         <v/>
       </c>
@@ -22569,10 +22569,10 @@
       <c r="J67" s="25" t="n"/>
       <c r="L67" s="25" t="n"/>
       <c r="M67" s="25" t="n"/>
-      <c r="O67" s="291" t="n"/>
+      <c r="O67" s="260" t="n"/>
       <c r="AD67" s="25" t="n"/>
       <c r="AG67" s="25" t="n"/>
-      <c r="AJ67" s="286" t="n"/>
+      <c r="AJ67" s="255" t="n"/>
       <c r="AK67" s="59">
         <f>Games!N36</f>
         <v/>
@@ -22591,7 +22591,7 @@
     </row>
     <row r="68" ht="15.6" customHeight="1">
       <c r="A68" s="13" t="n"/>
-      <c r="B68" s="286" t="n"/>
+      <c r="B68" s="255" t="n"/>
       <c r="C68" s="42" t="n"/>
       <c r="D68" s="72" t="n"/>
       <c r="F68" s="25" t="n"/>
@@ -22616,14 +22616,14 @@
       <c r="AG68" s="25" t="n"/>
       <c r="AJ68" s="25" t="n"/>
       <c r="AM68" s="25" t="n"/>
-      <c r="AN68" s="286" t="n"/>
-      <c r="AO68" s="277" t="n"/>
+      <c r="AN68" s="255" t="n"/>
+      <c r="AO68" s="287" t="n"/>
     </row>
     <row r="69" ht="15.6" customHeight="1">
       <c r="A69" s="13" t="n"/>
       <c r="C69" s="42" t="n"/>
       <c r="D69" s="72" t="n"/>
-      <c r="AO69" s="277" t="n"/>
+      <c r="AO69" s="287" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="258">
@@ -22631,55 +22631,55 @@
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="K63:K64"/>
+    <mergeCell ref="AH33:AH34"/>
     <mergeCell ref="AI65:AI66"/>
-    <mergeCell ref="AH33:AH34"/>
     <mergeCell ref="F55:F56"/>
     <mergeCell ref="AB59:AB60"/>
     <mergeCell ref="AH17:AH18"/>
     <mergeCell ref="AD59:AD60"/>
+    <mergeCell ref="F45:F46"/>
     <mergeCell ref="AI49:AI50"/>
-    <mergeCell ref="F45:F46"/>
     <mergeCell ref="AH53:AH54"/>
     <mergeCell ref="Y19:Y20"/>
     <mergeCell ref="H61:H62"/>
     <mergeCell ref="AJ13:AJ14"/>
+    <mergeCell ref="G65:G66"/>
     <mergeCell ref="J55:J56"/>
     <mergeCell ref="Y51:Y52"/>
-    <mergeCell ref="G65:G66"/>
     <mergeCell ref="AF55:AF56"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="K19:L20"/>
     <mergeCell ref="H45:H46"/>
-    <mergeCell ref="K19:L20"/>
-    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G49:G50"/>
     <mergeCell ref="S32:W33"/>
-    <mergeCell ref="G49:G50"/>
     <mergeCell ref="I43:I44"/>
+    <mergeCell ref="AI41:AI42"/>
     <mergeCell ref="AJ15:AJ16"/>
-    <mergeCell ref="AI41:AI42"/>
     <mergeCell ref="AO10:AO11"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F31:F32"/>
     <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H65:H66"/>
     <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H65:H66"/>
     <mergeCell ref="AH61:AH62"/>
     <mergeCell ref="AJ55:AJ56"/>
     <mergeCell ref="J47:J48"/>
     <mergeCell ref="AI25:AI26"/>
     <mergeCell ref="AG43:AG44"/>
     <mergeCell ref="F37:F38"/>
+    <mergeCell ref="AH45:AH46"/>
     <mergeCell ref="AF47:AF48"/>
     <mergeCell ref="H37:H38"/>
-    <mergeCell ref="AH45:AH46"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="AF7:AF8"/>
     <mergeCell ref="G41:G42"/>
     <mergeCell ref="AJ45:AJ46"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AO50:AO51"/>
     <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AO50:AO51"/>
     <mergeCell ref="AJ63:AJ64"/>
+    <mergeCell ref="AF31:AF32"/>
     <mergeCell ref="O19:O20"/>
-    <mergeCell ref="AF31:AF32"/>
     <mergeCell ref="AI5:AI6"/>
     <mergeCell ref="F57:F58"/>
     <mergeCell ref="AO34:AO35"/>
@@ -22687,32 +22687,33 @@
     <mergeCell ref="AJ47:AJ48"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="I15:I16"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="AH37:AH38"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="F63:F64"/>
+    <mergeCell ref="K55:K56"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="AH37:AH38"/>
-    <mergeCell ref="K55:K56"/>
     <mergeCell ref="M59:M60"/>
     <mergeCell ref="AG59:AG60"/>
     <mergeCell ref="AI53:AI54"/>
     <mergeCell ref="P51:P52"/>
     <mergeCell ref="AA19:AA20"/>
     <mergeCell ref="AE47:AE48"/>
+    <mergeCell ref="AJ17:AJ18"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="AJ17:AJ18"/>
+    <mergeCell ref="AG23:AG24"/>
     <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A54:A55"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A54:A55"/>
     <mergeCell ref="F5:F6"/>
+    <mergeCell ref="AE31:AE32"/>
     <mergeCell ref="H49:H50"/>
-    <mergeCell ref="AE31:AE32"/>
     <mergeCell ref="AG31:AG32"/>
     <mergeCell ref="L43:L44"/>
     <mergeCell ref="AO62:AO63"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="AI45:AI46"/>
     <mergeCell ref="O67:AA67"/>
-    <mergeCell ref="AI45:AI46"/>
-    <mergeCell ref="N43:N44"/>
     <mergeCell ref="V27:V28"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="AQ22:AQ27"/>
@@ -22721,13 +22722,13 @@
     <mergeCell ref="AH9:AH10"/>
     <mergeCell ref="AB43:AB44"/>
     <mergeCell ref="AO30:AO31"/>
+    <mergeCell ref="A46:A47"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="A46:A47"/>
     <mergeCell ref="AB27:AB28"/>
     <mergeCell ref="AE23:AE24"/>
     <mergeCell ref="AO14:AO15"/>
+    <mergeCell ref="M27:M28"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="M27:M28"/>
     <mergeCell ref="AO54:AO55"/>
     <mergeCell ref="AJ5:AJ6"/>
     <mergeCell ref="F9:F10"/>
@@ -22742,40 +22743,39 @@
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="AG63:AG64"/>
     <mergeCell ref="K51:L52"/>
+    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="V39:X40"/>
     <mergeCell ref="AJ29:AJ30"/>
-    <mergeCell ref="AH13:AH14"/>
     <mergeCell ref="M43:M44"/>
     <mergeCell ref="AH65:AH66"/>
-    <mergeCell ref="V39:X40"/>
     <mergeCell ref="AI33:AI34"/>
     <mergeCell ref="AJ21:AJ22"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="AJ31:AJ32"/>
+    <mergeCell ref="AO66:AO67"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="G61:G62"/>
-    <mergeCell ref="AO66:AO67"/>
     <mergeCell ref="F65:F66"/>
     <mergeCell ref="AH21:AH22"/>
     <mergeCell ref="AC43:AC44"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="AJ7:AJ8"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A6:A7"/>
     <mergeCell ref="AF63:AF64"/>
     <mergeCell ref="AJ23:AJ24"/>
+    <mergeCell ref="AO18:AO19"/>
     <mergeCell ref="AO58:AO59"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="AJ57:AJ58"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="AJ57:AJ58"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="AO18:AO19"/>
-    <mergeCell ref="AE7:AE8"/>
     <mergeCell ref="S2:W2"/>
     <mergeCell ref="I47:I48"/>
     <mergeCell ref="O66:AA66"/>
     <mergeCell ref="AD27:AD28"/>
+    <mergeCell ref="K47:K48"/>
     <mergeCell ref="F17:F18"/>
-    <mergeCell ref="K47:K48"/>
     <mergeCell ref="Q19:Q20"/>
     <mergeCell ref="AO42:AO43"/>
     <mergeCell ref="G37:G38"/>
@@ -22783,46 +22783,46 @@
     <mergeCell ref="F41:F42"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="K31:K32"/>
+    <mergeCell ref="AG7:AG8"/>
     <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AG7:AG8"/>
     <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="H57:H58"/>
     <mergeCell ref="AC59:AC60"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="P19:P20"/>
     <mergeCell ref="AH49:AH50"/>
-    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="AJ49:AJ50"/>
     <mergeCell ref="T11:V19"/>
-    <mergeCell ref="AJ49:AJ50"/>
-    <mergeCell ref="I39:I40"/>
     <mergeCell ref="AG47:AG48"/>
     <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="Z51:Z52"/>
     <mergeCell ref="R27:T28"/>
-    <mergeCell ref="Z51:Z52"/>
     <mergeCell ref="AJ33:AJ34"/>
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="AE55:AE56"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="AG55:AG56"/>
     <mergeCell ref="I23:I24"/>
-    <mergeCell ref="AG55:AG56"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="AI37:AI38"/>
     <mergeCell ref="N59:N60"/>
+    <mergeCell ref="AD19:AE20"/>
     <mergeCell ref="F49:F50"/>
+    <mergeCell ref="I63:I64"/>
     <mergeCell ref="L11:L12"/>
-    <mergeCell ref="I63:I64"/>
-    <mergeCell ref="AD19:AE20"/>
     <mergeCell ref="N11:N12"/>
+    <mergeCell ref="AO22:AO23"/>
     <mergeCell ref="F29:F30"/>
-    <mergeCell ref="AO22:AO23"/>
     <mergeCell ref="AG39:AG40"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="A38:A39"/>
+    <mergeCell ref="AA51:AA52"/>
     <mergeCell ref="H33:H34"/>
-    <mergeCell ref="AA51:AA52"/>
+    <mergeCell ref="AH25:AH26"/>
     <mergeCell ref="AI57:AI58"/>
-    <mergeCell ref="AH25:AH26"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="AJ25:AJ26"/>
     <mergeCell ref="AO46:AO47"/>
-    <mergeCell ref="AJ25:AJ26"/>
-    <mergeCell ref="T35:V35"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="AQ3:AQ11"/>
     <mergeCell ref="I27:I28"/>
@@ -22831,9 +22831,9 @@
     <mergeCell ref="AH5:AH6"/>
     <mergeCell ref="U27:U28"/>
     <mergeCell ref="G17:G18"/>
+    <mergeCell ref="AJ61:AJ62"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="G57:G58"/>
-    <mergeCell ref="AJ61:AJ62"/>
     <mergeCell ref="AF39:AF40"/>
     <mergeCell ref="AI9:AI10"/>
     <mergeCell ref="AG27:AG28"/>
@@ -22848,10 +22848,10 @@
     <mergeCell ref="Q51:Q52"/>
     <mergeCell ref="AH29:AH30"/>
     <mergeCell ref="AJ37:AJ38"/>
+    <mergeCell ref="K39:K40"/>
     <mergeCell ref="J7:J8"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="J63:J64"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="K39:K40"/>
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="AO26:AO27"/>
     <mergeCell ref="K23:K24"/>
@@ -22865,15 +22865,15 @@
     <mergeCell ref="AE15:AE16"/>
     <mergeCell ref="AO6:AO7"/>
     <mergeCell ref="AG15:AG16"/>
-    <mergeCell ref="A62:A63"/>
     <mergeCell ref="I59:I60"/>
     <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="AF23:AF24"/>
     <mergeCell ref="L27:L28"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="U39:U40"/>
+    <mergeCell ref="AI29:AI30"/>
     <mergeCell ref="N27:N28"/>
-    <mergeCell ref="U39:U40"/>
-    <mergeCell ref="AF23:AF24"/>
     <mergeCell ref="AH57:AH58"/>
-    <mergeCell ref="AI29:AI30"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="AD51:AE52"/>
@@ -22883,7 +22883,7 @@
     <mergeCell ref="AH41:AH42"/>
     <mergeCell ref="T39:T40"/>
     <mergeCell ref="AJ41:AJ42"/>
-    <mergeCell ref="AG23:AG24"/>
+    <mergeCell ref="AE7:AE8"/>
     <mergeCell ref="A30:A31"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>